<commit_message>
Solved Problems: Remove Duplicated Element from Sorted Array and Remove Element from Unsorted Array.
</commit_message>
<xml_diff>
--- a/LeetCode_Practice_Tracker_Aviral.xlsx
+++ b/LeetCode_Practice_Tracker_Aviral.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anilk\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Aviral\DSAInterviewPrep\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{808B1A6C-10EC-4691-A2F1-059B7A842EB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F3AB5A-9A48-46C9-9D89-4CB2D9764804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="52">
   <si>
     <t>ID</t>
   </si>
@@ -143,6 +143,39 @@
   </si>
   <si>
     <t>To Do</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>0(n)</t>
+  </si>
+  <si>
+    <t>O(n)</t>
+  </si>
+  <si>
+    <t>HashMap</t>
+  </si>
+  <si>
+    <t>Container With Most Water</t>
+  </si>
+  <si>
+    <t>O(1)</t>
+  </si>
+  <si>
+    <t>Two Pointers</t>
+  </si>
+  <si>
+    <t>O(n ^ 2)</t>
+  </si>
+  <si>
+    <t>3 Sum Closet</t>
+  </si>
+  <si>
+    <t>3 Sum</t>
+  </si>
+  <si>
+    <t>2 Sum</t>
   </si>
 </sst>
 </file>
@@ -201,10 +234,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -510,23 +549,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:C18"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.88671875" customWidth="1"/>
-    <col min="3" max="3" width="55.77734375" customWidth="1"/>
-    <col min="4" max="4" width="9.44140625" customWidth="1"/>
-    <col min="5" max="5" width="8.5546875" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" customWidth="1"/>
-    <col min="8" max="8" width="16.6640625" customWidth="1"/>
-    <col min="9" max="9" width="19.77734375" customWidth="1"/>
-    <col min="10" max="10" width="17.77734375" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="2"/>
+    <col min="2" max="2" width="14.88671875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="55.77734375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="9.44140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="8.5546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="19.77734375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="17.77734375" style="2" customWidth="1"/>
+    <col min="11" max="12" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -565,291 +604,407 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="3">
+        <v>45861</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="3">
+        <v>45861</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="3">
+        <v>45863</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" s="3">
+        <v>45863</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
+        <v>1</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C27" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D27" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="E27" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="2">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B28" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C28" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D28" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="E28" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B29" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C29" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D29" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="E29" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="2">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B30" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C30" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D30" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="E30" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="2">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B31" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C31" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D31" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="E31" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="2">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B32" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C32" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D32" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="E32" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="2">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B33" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C33" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D33" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="E33" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="2">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B34" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C34" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D34" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="E34" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="2">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B35" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C35" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D35" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="E35" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="2">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B36" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C36" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D36" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12">
+      <c r="E36" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="2">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B37" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C37" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D37" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13">
+      <c r="E37" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="2">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B38" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C38" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D38" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14">
+      <c r="E38" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="2">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B39" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C39" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D39" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15">
+      <c r="E39" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="2">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B40" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C40" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D40" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E15" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16">
+      <c r="E40" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="2">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B41" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C41" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D41" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17">
+      <c r="E41" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="2">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B42" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C42" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D42" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18">
+      <c r="E42" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="2">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B43" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C43" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D43" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E43" s="2" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Solved Problem: Insert Delete GetRandom in O(1) (Randomized Set) and Update Tracker Excel Sheet.
</commit_message>
<xml_diff>
--- a/LeetCode_Practice_Tracker_Aviral.xlsx
+++ b/LeetCode_Practice_Tracker_Aviral.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Aviral\DSAInterviewPrep\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F3AB5A-9A48-46C9-9D89-4CB2D9764804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F071E5B-39F9-426C-A485-1E9081C05827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="96" windowWidth="19356" windowHeight="12144" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="86">
   <si>
     <t>ID</t>
   </si>
@@ -176,6 +176,108 @@
   </si>
   <si>
     <t>2 Sum</t>
+  </si>
+  <si>
+    <t>Median of Two Sorted Array</t>
+  </si>
+  <si>
+    <t>Remove Duplicated from Sorted Array</t>
+  </si>
+  <si>
+    <t>Remove Element</t>
+  </si>
+  <si>
+    <t>Search In Rotated Sorted Array</t>
+  </si>
+  <si>
+    <t>Find First and Last Position of Element in Rotated Sorted Array</t>
+  </si>
+  <si>
+    <t>Search Insert Position</t>
+  </si>
+  <si>
+    <t>Rotate Image</t>
+  </si>
+  <si>
+    <t>Remove Duplicated from Sorted Array II</t>
+  </si>
+  <si>
+    <t>Search In Rotated Sorted Array II</t>
+  </si>
+  <si>
+    <t>Best Time to Buy and Sell Stock I</t>
+  </si>
+  <si>
+    <t>Best Time to Buy and Sell Stock II</t>
+  </si>
+  <si>
+    <t>Single Number</t>
+  </si>
+  <si>
+    <t>Find Minimum in Rotated Sorted Array</t>
+  </si>
+  <si>
+    <t>Find Minimum in Rotated Sorted Array II</t>
+  </si>
+  <si>
+    <t>Find Peak Element</t>
+  </si>
+  <si>
+    <t>Maximum Gap</t>
+  </si>
+  <si>
+    <t>Two Sum II</t>
+  </si>
+  <si>
+    <t>Largest Number</t>
+  </si>
+  <si>
+    <t>Rotate Array</t>
+  </si>
+  <si>
+    <t>Count Primes</t>
+  </si>
+  <si>
+    <t>Contains Duplicate</t>
+  </si>
+  <si>
+    <t>Contains Duplicate II</t>
+  </si>
+  <si>
+    <t>Product of Array Except Self</t>
+  </si>
+  <si>
+    <t>Missing Number</t>
+  </si>
+  <si>
+    <t>Move Zeros</t>
+  </si>
+  <si>
+    <t>Peeking Iterator</t>
+  </si>
+  <si>
+    <t>Find the Duplicate Number</t>
+  </si>
+  <si>
+    <t>Range Sum Query</t>
+  </si>
+  <si>
+    <t>Count of Smaller Numbers After Self</t>
+  </si>
+  <si>
+    <t>Top K Frequent Elements</t>
+  </si>
+  <si>
+    <t>Intersection of Two Arrays</t>
+  </si>
+  <si>
+    <t>Intersection of Two Arrays II</t>
+  </si>
+  <si>
+    <t>Insert Delete GetRandom in O(1) (Randomized Set)</t>
+  </si>
+  <si>
+    <t>Summary Ranges</t>
   </si>
 </sst>
 </file>
@@ -549,9 +651,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L43"/>
+  <dimension ref="A1:L62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -719,292 +823,699 @@
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>40</v>
+        <v>75</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>40</v>
+        <v>77</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>40</v>
+        <v>78</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>40</v>
+        <v>79</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>40</v>
+        <v>80</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>40</v>
+        <v>82</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>40</v>
+        <v>83</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
+        <v>41</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="2">
+        <v>1</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="2">
+        <v>2</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="2">
+        <v>3</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" s="2">
+        <v>4</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" s="2">
+        <v>5</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" s="2">
+        <v>6</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" s="2">
+        <v>7</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" s="2">
+        <v>8</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" s="2">
+        <v>9</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" s="2">
+        <v>10</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" s="2">
+        <v>11</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" s="2">
+        <v>12</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" s="2">
+        <v>13</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="C58" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" s="2">
+        <v>14</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" s="2">
+        <v>15</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61" s="2">
+        <v>16</v>
+      </c>
+      <c r="B61" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C61" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="D61" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E42" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" s="2">
+      <c r="E61" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62" s="2">
         <v>17</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B62" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C62" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="D62" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E43" s="2" t="s">
+      <c r="E62" s="2" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Solved Problem: Trapping Rain Water & Sort Colors.
</commit_message>
<xml_diff>
--- a/LeetCode_Practice_Tracker_Aviral.xlsx
+++ b/LeetCode_Practice_Tracker_Aviral.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Aviral\DSAInterviewPrep\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F071E5B-39F9-426C-A485-1E9081C05827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{031B7E53-3AB2-46B9-8CA9-BB4E6B3789DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="96" windowWidth="19356" windowHeight="12144" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="89">
   <si>
     <t>ID</t>
   </si>
@@ -49,9 +49,6 @@
     <t>Approach Summary</t>
   </si>
   <si>
-    <t>Code Link</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -278,6 +275,18 @@
   </si>
   <si>
     <t>Summary Ranges</t>
+  </si>
+  <si>
+    <t>Next Revision Date</t>
+  </si>
+  <si>
+    <t>Trapping Rain Water</t>
+  </si>
+  <si>
+    <t>Hard</t>
+  </si>
+  <si>
+    <t>Dutch Nation Flag Algo</t>
   </si>
 </sst>
 </file>
@@ -651,10 +660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L62"/>
+  <dimension ref="A1:L81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -701,10 +710,10 @@
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -712,28 +721,28 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F2" s="3">
         <v>45861</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -741,28 +750,28 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F3" s="3">
         <v>45861</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -770,28 +779,28 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F4" s="3">
         <v>45863</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -799,28 +808,28 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F5" s="3">
         <v>45863</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -828,10 +837,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -839,10 +851,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -850,10 +865,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -861,10 +879,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -872,10 +893,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -883,10 +907,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -894,10 +921,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -905,10 +935,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -916,10 +949,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -927,10 +963,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -938,585 +977,724 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C40" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A41" s="2">
+        <v>40</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="2">
-        <v>40</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E41" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A43" s="2">
+        <v>42</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F43" s="3">
+        <v>45882</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I43" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A44" s="2">
+        <v>43</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F44" s="3">
+        <v>45882</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65" s="2">
+        <v>1</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66" s="2">
+        <v>2</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67" s="2">
+        <v>3</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68" s="2">
+        <v>4</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A69" s="2">
+        <v>5</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70" s="2">
+        <v>6</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71" s="2">
+        <v>7</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A72" s="2">
+        <v>8</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A73" s="2">
+        <v>9</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A74" s="2">
+        <v>10</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A75" s="2">
+        <v>11</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A76" s="2">
+        <v>12</v>
+      </c>
+      <c r="B76" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C42" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="2">
-        <v>1</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D46" s="2" t="s">
+      <c r="C76" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A77" s="2">
+        <v>13</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A78" s="2">
+        <v>14</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A79" s="2">
+        <v>15</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A80" s="2">
+        <v>16</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A81" s="2">
+        <v>17</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D81" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E46" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="2">
-        <v>2</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D47" s="2" t="s">
+      <c r="E81" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="2">
-        <v>3</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" s="2">
-        <v>4</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" s="2">
-        <v>5</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" s="2">
-        <v>6</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52" s="2">
-        <v>7</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" s="2">
-        <v>8</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54" s="2">
-        <v>9</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A55" s="2">
-        <v>10</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A56" s="2">
-        <v>11</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A57" s="2">
-        <v>12</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A58" s="2">
-        <v>13</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" s="2">
-        <v>14</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" s="2">
-        <v>15</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A61" s="2">
-        <v>16</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A62" s="2">
-        <v>17</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Solved Problems: Group Anagrams, Insert Intervals and Merge Intervals.
</commit_message>
<xml_diff>
--- a/LeetCode_Practice_Tracker_Aviral.xlsx
+++ b/LeetCode_Practice_Tracker_Aviral.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Aviral\DSAInterviewPrep\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{031B7E53-3AB2-46B9-8CA9-BB4E6B3789DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52ACEA20-892A-48F1-BC01-C5C3B5466044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="96" windowWidth="19356" windowHeight="12144" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="102">
   <si>
     <t>ID</t>
   </si>
@@ -287,6 +287,45 @@
   </si>
   <si>
     <t>Dutch Nation Flag Algo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Array </t>
+  </si>
+  <si>
+    <t>First Missing Positive</t>
+  </si>
+  <si>
+    <t>Cycle Sort</t>
+  </si>
+  <si>
+    <t>Group Anagrams</t>
+  </si>
+  <si>
+    <t>O(NK)</t>
+  </si>
+  <si>
+    <t>Frequency Count + Map</t>
+  </si>
+  <si>
+    <t>Merged Intervals</t>
+  </si>
+  <si>
+    <t>O(n * log n)</t>
+  </si>
+  <si>
+    <t>Sorting</t>
+  </si>
+  <si>
+    <t>Insert Intervals</t>
+  </si>
+  <si>
+    <t>Normal Traversing</t>
+  </si>
+  <si>
+    <t>Gas Station</t>
+  </si>
+  <si>
+    <t>Candy</t>
   </si>
 </sst>
 </file>
@@ -662,8 +701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1408,6 +1447,132 @@
         <v>88</v>
       </c>
     </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45" s="2">
+        <v>44</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F45" s="3">
+        <v>45887</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A46" s="2">
+        <v>45</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F46" s="3">
+        <v>45887</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="I46" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A47" s="2">
+        <v>46</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F47" s="3">
+        <v>45889</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I47" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A48" s="2">
+        <v>47</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F48" s="3">
+        <v>45889</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C49" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C50" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
         <v>1</v>

</xml_diff>

<commit_message>
Solved Problem: Gas Station.
</commit_message>
<xml_diff>
--- a/LeetCode_Practice_Tracker_Aviral.xlsx
+++ b/LeetCode_Practice_Tracker_Aviral.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Aviral\DSAInterviewPrep\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52ACEA20-892A-48F1-BC01-C5C3B5466044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13DA1E73-9FBE-4F38-AB32-50BBE45FF226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="96" windowWidth="19356" windowHeight="12144" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="101">
   <si>
     <t>ID</t>
   </si>
@@ -323,9 +323,6 @@
   </si>
   <si>
     <t>Gas Station</t>
-  </si>
-  <si>
-    <t>Candy</t>
   </si>
 </sst>
 </file>
@@ -701,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1563,14 +1560,33 @@
         <v>99</v>
       </c>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A49" s="2">
+        <v>48</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="C49" s="2" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C50" s="2" t="s">
-        <v>101</v>
+      <c r="D49" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F49" s="3">
+        <v>45889</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Completed Revision of all array questions.
</commit_message>
<xml_diff>
--- a/LeetCode_Practice_Tracker_Aviral.xlsx
+++ b/LeetCode_Practice_Tracker_Aviral.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Aviral\DSAInterviewPrep\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13DA1E73-9FBE-4F38-AB32-50BBE45FF226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1FF4EF5-A4D1-4C08-8465-A2A8E72DE5AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="96" windowWidth="19356" windowHeight="12144" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="119">
   <si>
     <t>ID</t>
   </si>
@@ -223,9 +223,6 @@
     <t>Maximum Gap</t>
   </si>
   <si>
-    <t>Two Sum II</t>
-  </si>
-  <si>
     <t>Largest Number</t>
   </si>
   <si>
@@ -277,9 +274,6 @@
     <t>Summary Ranges</t>
   </si>
   <si>
-    <t>Next Revision Date</t>
-  </si>
-  <si>
     <t>Trapping Rain Water</t>
   </si>
   <si>
@@ -323,6 +317,66 @@
   </si>
   <si>
     <t>Gas Station</t>
+  </si>
+  <si>
+    <t>Last Revision Date</t>
+  </si>
+  <si>
+    <t>O(log n)</t>
+  </si>
+  <si>
+    <t>Binary Search</t>
+  </si>
+  <si>
+    <t>HashMap + Frequency</t>
+  </si>
+  <si>
+    <t>Hash Set</t>
+  </si>
+  <si>
+    <t>Hash Map</t>
+  </si>
+  <si>
+    <t>Prefix &amp; Suffix Product</t>
+  </si>
+  <si>
+    <t>Expected - Current Sum</t>
+  </si>
+  <si>
+    <t>Taking every min-max</t>
+  </si>
+  <si>
+    <t>XOR Every element</t>
+  </si>
+  <si>
+    <t>Using Two Pointers</t>
+  </si>
+  <si>
+    <t>Two Sum II - Input Array is Sorted</t>
+  </si>
+  <si>
+    <t>Convet String &amp; Sort</t>
+  </si>
+  <si>
+    <t>O(n log n)</t>
+  </si>
+  <si>
+    <t>Merge Sort</t>
+  </si>
+  <si>
+    <t>Need to repractice</t>
+  </si>
+  <si>
+    <t>Left - Question of Min Heap</t>
+  </si>
+  <si>
+    <t>O(n log k)</t>
+  </si>
+  <si>
+    <t>Floyd Cycle Detection</t>
+  </si>
+  <si>
+    <t>O(m + n)</t>
   </si>
 </sst>
 </file>
@@ -698,8 +752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+    <sheetView tabSelected="1" topLeftCell="B30" workbookViewId="0">
+      <selection activeCell="J47" sqref="J47:J48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -714,7 +768,8 @@
     <col min="8" max="8" width="16.6640625" style="2" customWidth="1"/>
     <col min="9" max="9" width="19.77734375" style="2" customWidth="1"/>
     <col min="10" max="10" width="17.77734375" style="2" customWidth="1"/>
-    <col min="11" max="12" width="8.88671875" style="2"/>
+    <col min="11" max="11" width="23.88671875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -746,7 +801,7 @@
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>9</v>
@@ -780,6 +835,9 @@
       <c r="I2" s="2" t="s">
         <v>43</v>
       </c>
+      <c r="J2" s="3">
+        <v>45894</v>
+      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
@@ -809,6 +867,9 @@
       <c r="I3" s="2" t="s">
         <v>46</v>
       </c>
+      <c r="J3" s="3">
+        <v>45894</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
@@ -878,8 +939,23 @@
       <c r="C6" s="2" t="s">
         <v>51</v>
       </c>
+      <c r="D6" s="2" t="s">
+        <v>85</v>
+      </c>
       <c r="E6" s="2" t="s">
         <v>40</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J6" s="3">
+        <v>45894</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -892,8 +968,20 @@
       <c r="C7" s="2" t="s">
         <v>52</v>
       </c>
+      <c r="D7" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="E7" s="2" t="s">
         <v>40</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J7" s="3">
+        <v>45891</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -906,8 +994,20 @@
       <c r="C8" s="2" t="s">
         <v>53</v>
       </c>
+      <c r="D8" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="E8" s="2" t="s">
         <v>40</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J8" s="3">
+        <v>45891</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -920,8 +1020,23 @@
       <c r="C9" s="2" t="s">
         <v>54</v>
       </c>
+      <c r="D9" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E9" s="2" t="s">
         <v>40</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="J9" s="3">
+        <v>45891</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -934,8 +1049,23 @@
       <c r="C10" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="D10" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E10" s="2" t="s">
         <v>40</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="J10" s="3">
+        <v>45891</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -948,8 +1078,23 @@
       <c r="C11" s="2" t="s">
         <v>56</v>
       </c>
+      <c r="D11" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="E11" s="2" t="s">
         <v>40</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="J11" s="3">
+        <v>45891</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -990,8 +1135,20 @@
       <c r="C14" s="2" t="s">
         <v>58</v>
       </c>
+      <c r="D14" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E14" s="2" t="s">
         <v>40</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J14" s="3">
+        <v>45891</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -1004,8 +1161,23 @@
       <c r="C15" s="2" t="s">
         <v>59</v>
       </c>
+      <c r="D15" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E15" s="2" t="s">
         <v>40</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="J15" s="3">
+        <v>45891</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -1018,11 +1190,23 @@
       <c r="C16" s="2" t="s">
         <v>60</v>
       </c>
+      <c r="D16" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="E16" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J16" s="3">
+        <v>45894</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1032,11 +1216,26 @@
       <c r="C17" s="2" t="s">
         <v>61</v>
       </c>
+      <c r="D17" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E17" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G17" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="J17" s="3">
+        <v>45894</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1046,11 +1245,26 @@
       <c r="C18" s="2" t="s">
         <v>62</v>
       </c>
+      <c r="D18" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="E18" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G18" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="J18" s="3">
+        <v>45894</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1060,11 +1274,26 @@
       <c r="C19" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="D19" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E19" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G19" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="J19" s="3">
+        <v>45891</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1074,11 +1303,26 @@
       <c r="C20" s="2" t="s">
         <v>64</v>
       </c>
+      <c r="D20" s="2" t="s">
+        <v>85</v>
+      </c>
       <c r="E20" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G20" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="J20" s="3">
+        <v>45891</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1088,11 +1332,23 @@
       <c r="C21" s="2" t="s">
         <v>65</v>
       </c>
+      <c r="D21" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E21" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G21" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J21" s="3">
+        <v>45891</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1102,11 +1358,23 @@
       <c r="C22" s="2" t="s">
         <v>66</v>
       </c>
+      <c r="D22" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E22" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G22" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J22" s="3">
+        <v>45894</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -1114,13 +1382,28 @@
         <v>13</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>67</v>
+        <v>110</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G23" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="J23" s="3">
+        <v>45894</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -1130,11 +1413,26 @@
       <c r="C24" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="D24" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="E24" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G24" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="J24" s="3">
+        <v>45891</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -1144,11 +1442,26 @@
       <c r="C25" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="D25" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E25" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G25" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="J25" s="3">
+        <v>45894</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -1156,13 +1469,28 @@
         <v>13</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G26" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="J26" s="3">
+        <v>45894</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -1170,13 +1498,25 @@
         <v>13</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G27" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J27" s="3">
+        <v>45891</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -1184,13 +1524,13 @@
         <v>13</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -1198,13 +1538,28 @@
         <v>13</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G29" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="J29" s="3">
+        <v>45894</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -1212,13 +1567,28 @@
         <v>13</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G30" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="J30" s="3">
+        <v>45894</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -1226,13 +1596,28 @@
         <v>13</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G31" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="J31" s="3">
+        <v>45894</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -1240,13 +1625,28 @@
         <v>13</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G32" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="J32" s="3">
+        <v>45894</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -1254,13 +1654,25 @@
         <v>13</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G33" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J33" s="3">
+        <v>45891</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -1268,13 +1680,13 @@
         <v>13</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -1282,13 +1694,28 @@
         <v>13</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G35" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="J35" s="3">
+        <v>45894</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -1296,13 +1723,13 @@
         <v>13</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -1310,13 +1737,31 @@
         <v>13</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G37" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="J37" s="3">
+        <v>45894</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -1324,27 +1769,54 @@
         <v>13</v>
       </c>
       <c r="C38" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A39" s="2">
+        <v>38</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E38" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="2">
-        <v>38</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>81</v>
+      <c r="D39" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G39" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="J39" s="3">
+        <v>45894</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -1352,27 +1824,42 @@
         <v>13</v>
       </c>
       <c r="C40" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="J40" s="3">
+        <v>45894</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A41" s="2">
+        <v>40</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E40" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="2">
-        <v>40</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>83</v>
-      </c>
       <c r="E41" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -1380,24 +1867,36 @@
         <v>13</v>
       </c>
       <c r="C42" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J42" s="3">
+        <v>45894</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A43" s="2">
+        <v>42</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E42" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="2">
-        <v>42</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="D43" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>40</v>
@@ -1414,8 +1913,11 @@
       <c r="I43" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J43" s="3">
+        <v>45894</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -1441,21 +1943,24 @@
         <v>45</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+      <c r="J44" s="3">
+        <v>45891</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>40</v>
@@ -1470,10 +1975,13 @@
         <v>45</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+      <c r="J45" s="3">
+        <v>45894</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -1481,7 +1989,7 @@
         <v>13</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>38</v>
@@ -1493,16 +2001,19 @@
         <v>45887</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+      <c r="J46" s="3">
+        <v>45894</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -1510,7 +2021,7 @@
         <v>13</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>38</v>
@@ -1522,16 +2033,19 @@
         <v>45889</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H47" s="2" t="s">
         <v>42</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+      <c r="J47" s="3">
+        <v>45894</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -1539,7 +2053,7 @@
         <v>13</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>38</v>
@@ -1557,10 +2071,13 @@
         <v>42</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+      <c r="J48" s="3">
+        <v>45894</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -1568,7 +2085,7 @@
         <v>13</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>38</v>
@@ -1586,7 +2103,10 @@
         <v>45</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
+      </c>
+      <c r="J49" s="3">
+        <v>45894</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved Problems: Longest Sub String without repeating characters, Maximum Size SubArray Sum & Find Max Average I.
</commit_message>
<xml_diff>
--- a/LeetCode_Practice_Tracker_Aviral.xlsx
+++ b/LeetCode_Practice_Tracker_Aviral.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Aviral\DSAInterviewPrep\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1FF4EF5-A4D1-4C08-8465-A2A8E72DE5AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{097D41EC-2935-4B9F-A0D9-2F0F6761B4FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="96" windowWidth="19356" windowHeight="12144" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="118">
   <si>
     <t>ID</t>
   </si>
@@ -109,12 +109,6 @@
     <t>Segregate 0s, 1s, and 2s</t>
   </si>
   <si>
-    <t>Two Sum</t>
-  </si>
-  <si>
-    <t>Best Time to Buy and Sell Stock</t>
-  </si>
-  <si>
     <t>Valid Anagram</t>
   </si>
   <si>
@@ -377,6 +371,9 @@
   </si>
   <si>
     <t>O(m + n)</t>
+  </si>
+  <si>
+    <t>Find Max Averga I</t>
   </si>
 </sst>
 </file>
@@ -752,8 +749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B30" workbookViewId="0">
-      <selection activeCell="J47" sqref="J47:J48"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="I53" sqref="I53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -801,7 +798,7 @@
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>9</v>
@@ -815,25 +812,25 @@
         <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F2" s="3">
         <v>45861</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="J2" s="3">
         <v>45894</v>
@@ -847,25 +844,25 @@
         <v>13</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F3" s="3">
         <v>45861</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J3" s="3">
         <v>45894</v>
@@ -879,25 +876,25 @@
         <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F4" s="3">
         <v>45863</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -908,25 +905,25 @@
         <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F5" s="3">
         <v>45863</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -937,22 +934,22 @@
         <v>13</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J6" s="3">
         <v>45894</v>
@@ -966,19 +963,19 @@
         <v>13</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J7" s="3">
         <v>45891</v>
@@ -992,19 +989,19 @@
         <v>13</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J8" s="3">
         <v>45891</v>
@@ -1018,22 +1015,22 @@
         <v>13</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J9" s="3">
         <v>45891</v>
@@ -1047,22 +1044,22 @@
         <v>13</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J10" s="3">
         <v>45891</v>
@@ -1076,22 +1073,22 @@
         <v>13</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J11" s="3">
         <v>45891</v>
@@ -1105,10 +1102,10 @@
         <v>13</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -1119,10 +1116,10 @@
         <v>13</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -1133,19 +1130,19 @@
         <v>13</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J14" s="3">
         <v>45891</v>
@@ -1159,22 +1156,22 @@
         <v>13</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J15" s="3">
         <v>45891</v>
@@ -1188,19 +1185,19 @@
         <v>13</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J16" s="3">
         <v>45894</v>
@@ -1214,22 +1211,22 @@
         <v>13</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="J17" s="3">
         <v>45894</v>
@@ -1243,22 +1240,22 @@
         <v>13</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="J18" s="3">
         <v>45894</v>
@@ -1272,22 +1269,22 @@
         <v>13</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J19" s="3">
         <v>45891</v>
@@ -1301,22 +1298,22 @@
         <v>13</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J20" s="3">
         <v>45891</v>
@@ -1330,19 +1327,19 @@
         <v>13</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J21" s="3">
         <v>45891</v>
@@ -1356,19 +1353,19 @@
         <v>13</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J22" s="3">
         <v>45894</v>
@@ -1382,22 +1379,22 @@
         <v>13</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="J23" s="3">
         <v>45894</v>
@@ -1414,19 +1411,19 @@
         <v>25</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J24" s="3">
         <v>45891</v>
@@ -1443,19 +1440,19 @@
         <v>26</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J25" s="3">
         <v>45894</v>
@@ -1469,22 +1466,22 @@
         <v>13</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="J26" s="3">
         <v>45894</v>
@@ -1498,19 +1495,19 @@
         <v>13</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J27" s="3">
         <v>45891</v>
@@ -1524,10 +1521,10 @@
         <v>13</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
@@ -1538,22 +1535,22 @@
         <v>13</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J29" s="3">
         <v>45894</v>
@@ -1567,22 +1564,22 @@
         <v>13</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J30" s="3">
         <v>45894</v>
@@ -1596,22 +1593,22 @@
         <v>13</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J31" s="3">
         <v>45894</v>
@@ -1625,22 +1622,22 @@
         <v>13</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J32" s="3">
         <v>45894</v>
@@ -1654,19 +1651,19 @@
         <v>13</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J33" s="3">
         <v>45891</v>
@@ -1680,10 +1677,10 @@
         <v>13</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
@@ -1694,22 +1691,22 @@
         <v>13</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="J35" s="3">
         <v>45894</v>
@@ -1723,10 +1720,10 @@
         <v>13</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
@@ -1737,28 +1734,28 @@
         <v>13</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="J37" s="3">
         <v>45894</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
@@ -1769,22 +1766,22 @@
         <v>13</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
@@ -1795,22 +1792,22 @@
         <v>13</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J39" s="3">
         <v>45894</v>
@@ -1824,22 +1821,22 @@
         <v>13</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J40" s="3">
         <v>45894</v>
@@ -1853,10 +1850,10 @@
         <v>13</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
@@ -1867,19 +1864,19 @@
         <v>13</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J42" s="3">
         <v>45894</v>
@@ -1893,25 +1890,25 @@
         <v>13</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F43" s="3">
         <v>45882</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J43" s="3">
         <v>45894</v>
@@ -1928,22 +1925,22 @@
         <v>27</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F44" s="3">
         <v>45882</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J44" s="3">
         <v>45891</v>
@@ -1954,28 +1951,28 @@
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F45" s="3">
         <v>45887</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J45" s="3">
         <v>45894</v>
@@ -1989,25 +1986,25 @@
         <v>13</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F46" s="3">
         <v>45887</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J46" s="3">
         <v>45894</v>
@@ -2021,25 +2018,25 @@
         <v>13</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F47" s="3">
         <v>45889</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J47" s="3">
         <v>45894</v>
@@ -2053,25 +2050,25 @@
         <v>13</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F48" s="3">
         <v>45889</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="J48" s="3">
         <v>45894</v>
@@ -2085,215 +2082,214 @@
         <v>13</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F49" s="3">
         <v>45889</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="J49" s="3">
         <v>45894</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A65" s="2">
-        <v>1</v>
-      </c>
-      <c r="B65" s="2" t="s">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A50" s="2">
+        <v>49</v>
+      </c>
+      <c r="B50" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C65" s="2" t="s">
+      <c r="C50" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D65" s="2" t="s">
+      <c r="D50" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E50" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E65" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A66" s="2">
-        <v>2</v>
-      </c>
-      <c r="B66" s="2" t="s">
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A51" s="2">
+        <v>50</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="C51" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D66" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E66" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A67" s="2">
-        <v>3</v>
-      </c>
-      <c r="B67" s="2" t="s">
+      <c r="D51" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F51" s="3">
+        <v>45896</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I51" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C67" s="2" t="s">
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A52" s="2">
+        <v>51</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D67" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A68" s="2">
-        <v>4</v>
-      </c>
-      <c r="B68" s="2" t="s">
+      <c r="D52" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F52" s="3">
+        <v>45896</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I52" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C68" s="2" t="s">
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A53" s="2">
+        <v>52</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F53" s="3">
+        <v>45896</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I53" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A54" s="2">
+        <v>53</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D68" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E68" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A69" s="2">
-        <v>5</v>
-      </c>
-      <c r="B69" s="2" t="s">
+      <c r="D54" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A55" s="2">
+        <v>54</v>
+      </c>
+      <c r="B55" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C69" s="2" t="s">
+      <c r="C55" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D69" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E69" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A70" s="2">
-        <v>6</v>
-      </c>
-      <c r="B70" s="2" t="s">
+      <c r="D55" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A56" s="2">
+        <v>55</v>
+      </c>
+      <c r="B56" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C70" s="2" t="s">
+      <c r="C56" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D70" s="2" t="s">
+      <c r="D56" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E56" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E70" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A71" s="2">
-        <v>7</v>
-      </c>
-      <c r="B71" s="2" t="s">
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A57" s="2">
+        <v>56</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C71" s="2" t="s">
+      <c r="C57" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D71" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E71" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A72" s="2">
-        <v>8</v>
-      </c>
-      <c r="B72" s="2" t="s">
+      <c r="D57" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B58" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C72" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E72" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A73" s="2">
-        <v>9</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C73" s="2" t="s">
+      <c r="C58" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D73" s="2" t="s">
+      <c r="D58" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E58" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="E73" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A74" s="2">
-        <v>10</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E74" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A75" s="2">
-        <v>11</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E75" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
@@ -2304,13 +2300,13 @@
         <v>14</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D76" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E76" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="E76" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
@@ -2321,13 +2317,13 @@
         <v>15</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D77" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E77" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="E77" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
@@ -2338,13 +2334,13 @@
         <v>16</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D78" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E78" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="E78" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
@@ -2355,13 +2351,13 @@
         <v>17</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D79" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E79" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="E79" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
@@ -2372,13 +2368,13 @@
         <v>18</v>
       </c>
       <c r="C80" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D80" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D80" s="2" t="s">
+      <c r="E80" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="E80" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
@@ -2389,13 +2385,13 @@
         <v>19</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Solved Problems: Repeated DNA Sequence & Longest Harmonious Sequence.
</commit_message>
<xml_diff>
--- a/LeetCode_Practice_Tracker_Aviral.xlsx
+++ b/LeetCode_Practice_Tracker_Aviral.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Aviral\DSAInterviewPrep\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{097D41EC-2935-4B9F-A0D9-2F0F6761B4FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0114B3D-877E-43FA-8AD9-20DFDD90E5CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="96" windowWidth="19356" windowHeight="12144" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="123">
   <si>
     <t>ID</t>
   </si>
@@ -374,6 +374,21 @@
   </si>
   <si>
     <t>Find Max Averga I</t>
+  </si>
+  <si>
+    <t>Repeated DNA Sequence</t>
+  </si>
+  <si>
+    <t>Set for seen &amp; repeated</t>
+  </si>
+  <si>
+    <t>O(10 * n)</t>
+  </si>
+  <si>
+    <t>Longest Harmonious Sequence</t>
+  </si>
+  <si>
+    <t>Using Frequency</t>
   </si>
 </sst>
 </file>
@@ -749,8 +764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="I53" sqref="I53"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="I56" sqref="I56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2218,13 +2233,25 @@
         <v>10</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>23</v>
+        <v>118</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="F54" s="3">
+        <v>45896</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="I54" s="2" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.3">
@@ -2235,13 +2262,25 @@
         <v>10</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>24</v>
+        <v>121</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="F55" s="3">
+        <v>45896</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I55" s="2" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.3">
@@ -2249,13 +2288,13 @@
         <v>55</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>37</v>
@@ -2266,10 +2305,10 @@
         <v>56</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>36</v>
@@ -2280,15 +2319,43 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B58" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>35</v>
       </c>
       <c r="E58" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B59" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B60" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E60" s="2" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Solved Problems: Sub Array Product Less Than K, Max Consecutive Ones III & Fruits Into Basket.
</commit_message>
<xml_diff>
--- a/LeetCode_Practice_Tracker_Aviral.xlsx
+++ b/LeetCode_Practice_Tracker_Aviral.xlsx
@@ -8,19 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Aviral\DSAInterviewPrep\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0114B3D-877E-43FA-8AD9-20DFDD90E5CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D940826-13B4-45F5-AD8F-B5A8CAA2ACE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="96" windowWidth="19356" windowHeight="12144" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="126">
   <si>
     <t>ID</t>
   </si>
@@ -389,6 +400,15 @@
   </si>
   <si>
     <t>Using Frequency</t>
+  </si>
+  <si>
+    <t>SubArray with Product Less then K</t>
+  </si>
+  <si>
+    <t>Max Consecutive Ones III</t>
+  </si>
+  <si>
+    <t>Fruits Into Basket</t>
   </si>
 </sst>
 </file>
@@ -765,7 +785,7 @@
   <dimension ref="A1:L81"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="I56" sqref="I56"/>
+      <selection activeCell="E58" sqref="E58:I58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2291,13 +2311,25 @@
         <v>10</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>23</v>
+        <v>123</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="F56" s="3">
+        <v>45898</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I56" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.3">
@@ -2308,55 +2340,154 @@
         <v>10</v>
       </c>
       <c r="C57" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F57" s="3">
+        <v>45898</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I57" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A58" s="2">
+        <v>57</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F58" s="3">
+        <v>45898</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I58" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A59" s="2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A60" s="2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A61" s="2">
+        <v>60</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A62" s="2">
+        <v>61</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C62" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D57" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E57" s="2" t="s">
+      <c r="D62" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E62" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B58" s="2" t="s">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A63" s="2">
+        <v>62</v>
+      </c>
+      <c r="B63" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="C63" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D58" s="2" t="s">
+      <c r="D63" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E58" s="2" t="s">
+      <c r="E63" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B59" s="2" t="s">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A64" s="2">
+        <v>63</v>
+      </c>
+      <c r="B64" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="C64" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D59" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E59" s="2" t="s">
+      <c r="D64" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E64" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B60" s="2" t="s">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65" s="2">
+        <v>64</v>
+      </c>
+      <c r="B65" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="C65" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D60" s="2" t="s">
+      <c r="D65" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E60" s="2" t="s">
+      <c r="E65" s="2" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66" s="2">
+        <v>65</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved Problems: Permutation in String.
</commit_message>
<xml_diff>
--- a/LeetCode_Practice_Tracker_Aviral.xlsx
+++ b/LeetCode_Practice_Tracker_Aviral.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Aviral\DSAInterviewPrep\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D940826-13B4-45F5-AD8F-B5A8CAA2ACE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA956847-C9C4-4F28-922B-07346C7AD3AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="96" windowWidth="19356" windowHeight="12144" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="128">
   <si>
     <t>ID</t>
   </si>
@@ -409,6 +409,12 @@
   </si>
   <si>
     <t>Fruits Into Basket</t>
+  </si>
+  <si>
+    <t>Permutaion in String</t>
+  </si>
+  <si>
+    <t>Sliding Window + Hmap</t>
   </si>
 </sst>
 </file>
@@ -784,8 +790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="E58" sqref="E58:I58"/>
+    <sheetView tabSelected="1" topLeftCell="B41" workbookViewId="0">
+      <selection activeCell="I60" sqref="I60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2394,6 +2400,30 @@
       <c r="A59" s="2">
         <v>58</v>
       </c>
+      <c r="B59" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F59" s="3">
+        <v>45899</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I59" s="2" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" s="2">

</xml_diff>

<commit_message>
Solved Problems: Find All Anagrams in a String & Longest Repeating Character Replacement.
</commit_message>
<xml_diff>
--- a/LeetCode_Practice_Tracker_Aviral.xlsx
+++ b/LeetCode_Practice_Tracker_Aviral.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Aviral\DSAInterviewPrep\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA956847-C9C4-4F28-922B-07346C7AD3AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE0A4DE-F20C-412C-8338-8CB93210BE09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="96" windowWidth="19356" windowHeight="12144" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="130">
   <si>
     <t>ID</t>
   </si>
@@ -415,6 +415,12 @@
   </si>
   <si>
     <t>Sliding Window + Hmap</t>
+  </si>
+  <si>
+    <t>Find All Anagrams In a String</t>
+  </si>
+  <si>
+    <t>Longest Repeating Character Replacement</t>
   </si>
 </sst>
 </file>
@@ -790,8 +796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B41" workbookViewId="0">
-      <selection activeCell="I60" sqref="I60"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61:I61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2429,6 +2435,30 @@
       <c r="A60" s="2">
         <v>59</v>
       </c>
+      <c r="B60" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F60" s="3">
+        <v>45899</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I60" s="2" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
@@ -2438,58 +2468,46 @@
         <v>10</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>23</v>
+        <v>129</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="F61" s="3">
+        <v>45899</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I61" s="2" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <v>61</v>
       </c>
-      <c r="B62" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
         <v>62</v>
       </c>
-      <c r="B63" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E63" s="2" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
         <v>63</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>36</v>
@@ -2503,13 +2521,13 @@
         <v>64</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>37</v>
@@ -2518,6 +2536,67 @@
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
         <v>65</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67" s="2">
+        <v>66</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68" s="2">
+        <v>67</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A69" s="2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70" s="2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71" s="2">
+        <v>70</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved Problems: Sub Arrays with K Distinct Elements and Binary Sub Array with Sum.
</commit_message>
<xml_diff>
--- a/LeetCode_Practice_Tracker_Aviral.xlsx
+++ b/LeetCode_Practice_Tracker_Aviral.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Aviral\DSAInterviewPrep\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE0A4DE-F20C-412C-8338-8CB93210BE09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76734320-165C-4E15-B44B-7124DF2E6EDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="96" windowWidth="19356" windowHeight="12144" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="135">
   <si>
     <t>ID</t>
   </si>
@@ -421,6 +421,21 @@
   </si>
   <si>
     <t>Longest Repeating Character Replacement</t>
+  </si>
+  <si>
+    <t>Subarrays with K Different Integers</t>
+  </si>
+  <si>
+    <t>Binary Subarrays With Sum</t>
+  </si>
+  <si>
+    <t>Minimum Window Substring</t>
+  </si>
+  <si>
+    <t>Sliding Window Maximum</t>
+  </si>
+  <si>
+    <t>Longest Substring with At Least K Repeating Characters</t>
   </si>
 </sst>
 </file>
@@ -796,8 +811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61:I61"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="H64" sqref="H64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2493,11 +2508,59 @@
       <c r="A62" s="2">
         <v>61</v>
       </c>
+      <c r="B62" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F62" s="3">
+        <v>45901</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I62" s="2" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
         <v>62</v>
       </c>
+      <c r="B63" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F63" s="3">
+        <v>45901</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I63" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
@@ -2507,13 +2570,7 @@
         <v>10</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E64" s="2" t="s">
-        <v>37</v>
+        <v>132</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
@@ -2524,65 +2581,26 @@
         <v>10</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E65" s="2" t="s">
-        <v>37</v>
+        <v>133</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
         <v>65</v>
       </c>
-      <c r="B66" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="C66" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E66" s="2" t="s">
-        <v>37</v>
+        <v>134</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
         <v>66</v>
       </c>
-      <c r="B67" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
         <v>67</v>
       </c>
-      <c r="B68" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D68" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E68" s="2" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="2">
@@ -2593,10 +2611,76 @@
       <c r="A70" s="2">
         <v>69</v>
       </c>
+      <c r="B70" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="2">
         <v>70</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B72" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B73" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B74" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved Problem: Minimum Window Sub String.
</commit_message>
<xml_diff>
--- a/LeetCode_Practice_Tracker_Aviral.xlsx
+++ b/LeetCode_Practice_Tracker_Aviral.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Aviral\DSAInterviewPrep\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76734320-165C-4E15-B44B-7124DF2E6EDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB29508-DA1D-4E94-968A-FB62DB00200C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="96" windowWidth="19356" windowHeight="12144" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="136">
   <si>
     <t>ID</t>
   </si>
@@ -436,6 +436,9 @@
   </si>
   <si>
     <t>Longest Substring with At Least K Repeating Characters</t>
+  </si>
+  <si>
+    <t>Sliding Window + Freq</t>
   </si>
 </sst>
 </file>
@@ -812,7 +815,7 @@
   <dimension ref="A1:L81"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="H64" sqref="H64"/>
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2572,6 +2575,24 @@
       <c r="C64" s="2" t="s">
         <v>132</v>
       </c>
+      <c r="D64" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F64" s="3">
+        <v>45902</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H64" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I64" s="2" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
@@ -2587,6 +2608,9 @@
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
         <v>65</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>134</v>

</xml_diff>

<commit_message>
Solved Problems: Maximum Sliding Window & Longest SubString with At Least K Repeating Characters.
</commit_message>
<xml_diff>
--- a/LeetCode_Practice_Tracker_Aviral.xlsx
+++ b/LeetCode_Practice_Tracker_Aviral.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Aviral\DSAInterviewPrep\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB29508-DA1D-4E94-968A-FB62DB00200C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33D8D8B4-75B9-4FC5-9EEA-7CF30820A9FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="96" windowWidth="19356" windowHeight="12144" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="135">
   <si>
     <t>ID</t>
   </si>
@@ -93,21 +93,12 @@
     <t>Matrix</t>
   </si>
   <si>
-    <t>Maximum Sum Subarray of Size K</t>
-  </si>
-  <si>
     <t>Longest Substring Without Repeating Characters</t>
   </si>
   <si>
     <t>Minimum Size Subarray Sum</t>
   </si>
   <si>
-    <t>First Negative Integer in Every Window of Size K</t>
-  </si>
-  <si>
-    <t>Count Occurrences of Anagrams</t>
-  </si>
-  <si>
     <t>Majority Element</t>
   </si>
   <si>
@@ -384,9 +375,6 @@
     <t>O(m + n)</t>
   </si>
   <si>
-    <t>Find Max Averga I</t>
-  </si>
-  <si>
     <t>Repeated DNA Sequence</t>
   </si>
   <si>
@@ -439,6 +427,15 @@
   </si>
   <si>
     <t>Sliding Window + Freq</t>
+  </si>
+  <si>
+    <t>Sliding Window + Deque</t>
+  </si>
+  <si>
+    <t>Find Max Average I</t>
+  </si>
+  <si>
+    <t>Divide &amp; Conquer</t>
   </si>
 </sst>
 </file>
@@ -814,7 +811,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
       <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
@@ -828,7 +825,7 @@
     <col min="6" max="6" width="12.44140625" style="2" customWidth="1"/>
     <col min="7" max="7" width="15.33203125" style="2" customWidth="1"/>
     <col min="8" max="8" width="16.6640625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="19.77734375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="21" style="2" customWidth="1"/>
     <col min="10" max="10" width="17.77734375" style="2" customWidth="1"/>
     <col min="11" max="11" width="23.88671875" style="2" customWidth="1"/>
     <col min="12" max="12" width="8.88671875" style="2"/>
@@ -863,7 +860,7 @@
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>9</v>
@@ -877,25 +874,25 @@
         <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F2" s="3">
         <v>45861</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="J2" s="3">
         <v>45894</v>
@@ -909,25 +906,25 @@
         <v>13</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F3" s="3">
         <v>45861</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="J3" s="3">
         <v>45894</v>
@@ -941,25 +938,25 @@
         <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F4" s="3">
         <v>45863</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -970,25 +967,25 @@
         <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F5" s="3">
         <v>45863</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -999,22 +996,22 @@
         <v>13</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="J6" s="3">
         <v>45894</v>
@@ -1028,19 +1025,19 @@
         <v>13</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="J7" s="3">
         <v>45891</v>
@@ -1054,19 +1051,19 @@
         <v>13</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="J8" s="3">
         <v>45891</v>
@@ -1080,22 +1077,22 @@
         <v>13</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="J9" s="3">
         <v>45891</v>
@@ -1109,22 +1106,22 @@
         <v>13</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="J10" s="3">
         <v>45891</v>
@@ -1138,22 +1135,22 @@
         <v>13</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="J11" s="3">
         <v>45891</v>
@@ -1167,10 +1164,10 @@
         <v>13</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -1181,10 +1178,10 @@
         <v>13</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -1195,19 +1192,19 @@
         <v>13</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="J14" s="3">
         <v>45891</v>
@@ -1221,22 +1218,22 @@
         <v>13</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="J15" s="3">
         <v>45891</v>
@@ -1250,19 +1247,19 @@
         <v>13</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="J16" s="3">
         <v>45894</v>
@@ -1276,22 +1273,22 @@
         <v>13</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="J17" s="3">
         <v>45894</v>
@@ -1305,22 +1302,22 @@
         <v>13</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="J18" s="3">
         <v>45894</v>
@@ -1334,22 +1331,22 @@
         <v>13</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="J19" s="3">
         <v>45891</v>
@@ -1363,22 +1360,22 @@
         <v>13</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="J20" s="3">
         <v>45891</v>
@@ -1392,19 +1389,19 @@
         <v>13</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="J21" s="3">
         <v>45891</v>
@@ -1418,19 +1415,19 @@
         <v>13</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="J22" s="3">
         <v>45894</v>
@@ -1444,22 +1441,22 @@
         <v>13</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="J23" s="3">
         <v>45894</v>
@@ -1473,22 +1470,22 @@
         <v>13</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J24" s="3">
         <v>45891</v>
@@ -1502,22 +1499,22 @@
         <v>13</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J25" s="3">
         <v>45894</v>
@@ -1531,22 +1528,22 @@
         <v>13</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="J26" s="3">
         <v>45894</v>
@@ -1560,19 +1557,19 @@
         <v>13</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="J27" s="3">
         <v>45891</v>
@@ -1586,10 +1583,10 @@
         <v>13</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
@@ -1600,22 +1597,22 @@
         <v>13</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="J29" s="3">
         <v>45894</v>
@@ -1629,22 +1626,22 @@
         <v>13</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="J30" s="3">
         <v>45894</v>
@@ -1658,22 +1655,22 @@
         <v>13</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="J31" s="3">
         <v>45894</v>
@@ -1687,22 +1684,22 @@
         <v>13</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="J32" s="3">
         <v>45894</v>
@@ -1716,19 +1713,19 @@
         <v>13</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="J33" s="3">
         <v>45891</v>
@@ -1742,10 +1739,10 @@
         <v>13</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
@@ -1756,22 +1753,22 @@
         <v>13</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="J35" s="3">
         <v>45894</v>
@@ -1785,10 +1782,10 @@
         <v>13</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
@@ -1799,28 +1796,28 @@
         <v>13</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="J37" s="3">
         <v>45894</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
@@ -1831,22 +1828,22 @@
         <v>13</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
@@ -1857,22 +1854,22 @@
         <v>13</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="J39" s="3">
         <v>45894</v>
@@ -1886,22 +1883,22 @@
         <v>13</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="J40" s="3">
         <v>45894</v>
@@ -1915,10 +1912,10 @@
         <v>13</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
@@ -1929,19 +1926,19 @@
         <v>13</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="J42" s="3">
         <v>45894</v>
@@ -1955,25 +1952,25 @@
         <v>13</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F43" s="3">
         <v>45882</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="J43" s="3">
         <v>45894</v>
@@ -1987,25 +1984,25 @@
         <v>13</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F44" s="3">
         <v>45882</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="J44" s="3">
         <v>45891</v>
@@ -2016,28 +2013,28 @@
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F45" s="3">
         <v>45887</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="J45" s="3">
         <v>45894</v>
@@ -2051,25 +2048,25 @@
         <v>13</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F46" s="3">
         <v>45887</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J46" s="3">
         <v>45894</v>
@@ -2083,25 +2080,25 @@
         <v>13</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F47" s="3">
         <v>45889</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="J47" s="3">
         <v>45894</v>
@@ -2115,25 +2112,25 @@
         <v>13</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F48" s="3">
         <v>45889</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="J48" s="3">
         <v>45894</v>
@@ -2147,25 +2144,25 @@
         <v>13</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F49" s="3">
         <v>45889</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="J49" s="3">
         <v>45894</v>
@@ -2182,10 +2179,22 @@
         <v>20</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
+      </c>
+      <c r="F50" s="3">
+        <v>45896</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I50" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
@@ -2199,16 +2208,16 @@
         <v>21</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F51" s="3">
         <v>45896</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H51" s="2" t="s">
         <v>40</v>
@@ -2225,22 +2234,22 @@
         <v>10</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>22</v>
+        <v>133</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F52" s="3">
         <v>45896</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I52" s="2" t="s">
         <v>10</v>
@@ -2254,25 +2263,25 @@
         <v>10</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F53" s="3">
         <v>45896</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>40</v>
+        <v>116</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>43</v>
+        <v>116</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>10</v>
+        <v>115</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.3">
@@ -2283,25 +2292,25 @@
         <v>10</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F54" s="3">
         <v>45896</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>120</v>
+        <v>37</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>120</v>
+        <v>37</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.3">
@@ -2312,25 +2321,25 @@
         <v>10</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F55" s="3">
-        <v>45896</v>
+        <v>45898</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H55" s="2" t="s">
         <v>40</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>122</v>
+        <v>10</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.3">
@@ -2341,22 +2350,22 @@
         <v>10</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F56" s="3">
         <v>45898</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I56" s="2" t="s">
         <v>10</v>
@@ -2370,22 +2379,22 @@
         <v>10</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F57" s="3">
         <v>45898</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I57" s="2" t="s">
         <v>10</v>
@@ -2399,25 +2408,25 @@
         <v>10</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F58" s="3">
-        <v>45898</v>
+        <v>45899</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>10</v>
+        <v>123</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.3">
@@ -2428,25 +2437,25 @@
         <v>10</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F59" s="3">
         <v>45899</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.3">
@@ -2457,25 +2466,25 @@
         <v>10</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F60" s="3">
         <v>45899</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I60" s="2" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.3">
@@ -2486,25 +2495,25 @@
         <v>10</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F61" s="3">
-        <v>45899</v>
+        <v>45901</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="I61" s="2" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.3">
@@ -2515,25 +2524,25 @@
         <v>10</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F62" s="3">
         <v>45901</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H62" s="2" t="s">
         <v>40</v>
       </c>
       <c r="I62" s="2" t="s">
-        <v>127</v>
+        <v>10</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.3">
@@ -2544,25 +2553,25 @@
         <v>10</v>
       </c>
       <c r="C63" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F63" s="3">
+        <v>45902</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I63" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E63" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F63" s="3">
-        <v>45901</v>
-      </c>
-      <c r="G63" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H63" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I63" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.3">
@@ -2573,240 +2582,210 @@
         <v>10</v>
       </c>
       <c r="C64" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F64" s="3">
+        <v>45903</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H64" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I64" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="D64" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E64" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F64" s="3">
-        <v>45902</v>
-      </c>
-      <c r="G64" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H64" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I64" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
         <v>64</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>10</v>
+        <v>134</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F65" s="3">
+        <v>45903</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H65" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I65" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
         <v>65</v>
       </c>
-      <c r="B66" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" s="2">
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" s="2">
         <v>69</v>
       </c>
-      <c r="B70" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E70" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" s="2">
         <v>70</v>
       </c>
-      <c r="B71" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E71" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B72" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E72" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B73" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B74" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B75" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C74" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E74" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A76" s="2">
-        <v>12</v>
-      </c>
+      <c r="C75" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B76" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A77" s="2">
-        <v>13</v>
-      </c>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B77" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A78" s="2">
-        <v>14</v>
-      </c>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B78" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A79" s="2">
-        <v>15</v>
-      </c>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B79" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C79" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D79" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D79" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="E79" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A80" s="2">
-        <v>16</v>
-      </c>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B80" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A81" s="2">
-        <v>17</v>
-      </c>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="81" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B81" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C81" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E81" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="D81" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E81" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Solved Problems: Running Sum of 1D Array, Find Pivot Index & SubArray Sum Equals K using Prefix Sum Technique.
</commit_message>
<xml_diff>
--- a/LeetCode_Practice_Tracker_Aviral.xlsx
+++ b/LeetCode_Practice_Tracker_Aviral.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Aviral\DSAInterviewPrep\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33D8D8B4-75B9-4FC5-9EEA-7CF30820A9FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51313CA0-FC9D-450E-BADF-8F4E1DC426DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="96" windowWidth="19356" windowHeight="12144" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="141">
   <si>
     <t>ID</t>
   </si>
@@ -436,6 +436,24 @@
   </si>
   <si>
     <t>Divide &amp; Conquer</t>
+  </si>
+  <si>
+    <t>Prefix Sum</t>
+  </si>
+  <si>
+    <t>Running Sum of 1d Array</t>
+  </si>
+  <si>
+    <t>Find Pivot Index</t>
+  </si>
+  <si>
+    <t>Subarray Sum Equals K</t>
+  </si>
+  <si>
+    <t>Range Sum Query – Immutable</t>
+  </si>
+  <si>
+    <t>Prefix Sum + HashMap</t>
   </si>
 </sst>
 </file>
@@ -811,8 +829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="G70" sqref="G70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2636,20 +2654,113 @@
       <c r="A66" s="2">
         <v>65</v>
       </c>
+      <c r="B66" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F66" s="3">
+        <v>45910</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H66" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I66" s="2" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
         <v>66</v>
       </c>
+      <c r="B67" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F67" s="3">
+        <v>45910</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H67" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I67" s="2" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
         <v>67</v>
       </c>
+      <c r="B68" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F68" s="3">
+        <v>45910</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H68" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I68" s="2" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" s="2">
         <v>68</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H69" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I69" s="2" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved Problems: Continuous Sub Array Sum, Sub Array Sum Divisible By K and Range Sum Query 2D - Immutable.
</commit_message>
<xml_diff>
--- a/LeetCode_Practice_Tracker_Aviral.xlsx
+++ b/LeetCode_Practice_Tracker_Aviral.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Aviral\DSAInterviewPrep\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51313CA0-FC9D-450E-BADF-8F4E1DC426DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C9425B5-2EDA-406A-8951-307B67D957F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="96" windowWidth="19356" windowHeight="12144" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="145">
   <si>
     <t>ID</t>
   </si>
@@ -454,6 +454,18 @@
   </si>
   <si>
     <t>Prefix Sum + HashMap</t>
+  </si>
+  <si>
+    <t>Continuous Subarray Sum</t>
+  </si>
+  <si>
+    <t>Subarray Sum Divisible by K</t>
+  </si>
+  <si>
+    <t>Range Sum Query 2D - Immutable</t>
+  </si>
+  <si>
+    <t>O(m * n)</t>
   </si>
 </sst>
 </file>
@@ -827,10 +839,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L81"/>
+  <dimension ref="A1:L94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="G70" sqref="G70"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="G72" sqref="G72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2767,139 +2779,267 @@
       <c r="A70" s="2">
         <v>69</v>
       </c>
+      <c r="B70" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F70" s="3">
+        <v>45912</v>
+      </c>
+      <c r="G70" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H70" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I70" s="2" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" s="2">
         <v>70</v>
       </c>
+      <c r="B71" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F71" s="3">
+        <v>45912</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H71" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I71" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A72" s="2">
+        <v>71</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F72" s="3">
+        <v>45912</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H72" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I72" s="2" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B73" s="2" t="s">
+      <c r="A73" s="2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A74" s="2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A75" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A76" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A77" s="2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A78" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A79" s="2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A80" s="2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A81" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A82" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B86" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C73" s="2" t="s">
+      <c r="C86" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D73" s="2" t="s">
+      <c r="D86" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E73" s="2" t="s">
+      <c r="E86" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B74" s="2" t="s">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B87" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C74" s="2" t="s">
+      <c r="C87" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D74" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E74" s="2" t="s">
+      <c r="D87" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E87" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B75" s="2" t="s">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B88" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C75" s="2" t="s">
+      <c r="C88" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D75" s="2" t="s">
+      <c r="D88" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E75" s="2" t="s">
+      <c r="E88" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B76" s="2" t="s">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B89" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="C89" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D76" s="2" t="s">
+      <c r="D89" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E76" s="2" t="s">
+      <c r="E89" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B77" s="2" t="s">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B90" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C77" s="2" t="s">
+      <c r="C90" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D77" s="2" t="s">
+      <c r="D90" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E77" s="2" t="s">
+      <c r="E90" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B78" s="2" t="s">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B91" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C78" s="2" t="s">
+      <c r="C91" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D78" s="2" t="s">
+      <c r="D91" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E78" s="2" t="s">
+      <c r="E91" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B79" s="2" t="s">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B92" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C79" s="2" t="s">
+      <c r="C92" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D79" s="2" t="s">
+      <c r="D92" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E79" s="2" t="s">
+      <c r="E92" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B80" s="2" t="s">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B93" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C80" s="2" t="s">
+      <c r="C93" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D80" s="2" t="s">
+      <c r="D93" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E80" s="2" t="s">
+      <c r="E93" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B81" s="2" t="s">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B94" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C81" s="2" t="s">
+      <c r="C94" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D81" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E81" s="2" t="s">
+      <c r="D94" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E94" s="2" t="s">
         <v>34</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Solved Problem: Matrix Block Sum.
</commit_message>
<xml_diff>
--- a/LeetCode_Practice_Tracker_Aviral.xlsx
+++ b/LeetCode_Practice_Tracker_Aviral.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Aviral\DSAInterviewPrep\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C9425B5-2EDA-406A-8951-307B67D957F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EF5126A-32C1-4D27-84FC-516ACFC2C525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="96" windowWidth="19356" windowHeight="12144" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="146">
   <si>
     <t>ID</t>
   </si>
@@ -466,6 +466,9 @@
   </si>
   <si>
     <t>O(m * n)</t>
+  </si>
+  <si>
+    <t>Matrix Block Sum</t>
   </si>
 </sst>
 </file>
@@ -842,7 +845,7 @@
   <dimension ref="A1:L94"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="G72" sqref="G72"/>
+      <selection activeCell="D73" sqref="D73:I73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2866,6 +2869,30 @@
       <c r="A73" s="2">
         <v>72</v>
       </c>
+      <c r="B73" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F73" s="3">
+        <v>45912</v>
+      </c>
+      <c r="G73" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H73" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I73" s="2" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" s="2">

</xml_diff>

<commit_message>
Solved Problems: Count Number of Nice Sub Arrays and Minimum Operations to Reduce X to Zero.
</commit_message>
<xml_diff>
--- a/LeetCode_Practice_Tracker_Aviral.xlsx
+++ b/LeetCode_Practice_Tracker_Aviral.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Aviral\DSAInterviewPrep\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EF5126A-32C1-4D27-84FC-516ACFC2C525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6FAEAD4-B0C9-4672-B36D-335309F37779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="96" windowWidth="19356" windowHeight="12144" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="148">
   <si>
     <t>ID</t>
   </si>
@@ -469,6 +469,12 @@
   </si>
   <si>
     <t>Matrix Block Sum</t>
+  </si>
+  <si>
+    <t>Count Number of Nice Sub Arrays</t>
+  </si>
+  <si>
+    <t>Minimum Operations to Reduce X to Zero</t>
   </si>
 </sst>
 </file>
@@ -845,7 +851,7 @@
   <dimension ref="A1:L94"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="D73" sqref="D73:I73"/>
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2898,10 +2904,58 @@
       <c r="A74" s="2">
         <v>73</v>
       </c>
+      <c r="B74" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F74" s="3">
+        <v>45914</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H74" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I74" s="2" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" s="2">
         <v>74</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F75" s="3">
+        <v>45914</v>
+      </c>
+      <c r="G75" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H75" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I75" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved Problems: Maximum Size Sub Array Sum, Maximum SubArray and Maximum Sum Circular Sub Array.
</commit_message>
<xml_diff>
--- a/LeetCode_Practice_Tracker_Aviral.xlsx
+++ b/LeetCode_Practice_Tracker_Aviral.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Aviral\DSAInterviewPrep\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6FAEAD4-B0C9-4672-B36D-335309F37779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACBA08B6-B53A-4C80-B0A8-675DE6CF2E07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="96" windowWidth="19356" windowHeight="12144" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="153">
   <si>
     <t>ID</t>
   </si>
@@ -475,6 +475,21 @@
   </si>
   <si>
     <t>Minimum Operations to Reduce X to Zero</t>
+  </si>
+  <si>
+    <t>Maximum Size Subarray Sum Equals K</t>
+  </si>
+  <si>
+    <t>Maximum Subarray</t>
+  </si>
+  <si>
+    <t>Maximum Sum Circular Subarray</t>
+  </si>
+  <si>
+    <t>Kadane Algo</t>
+  </si>
+  <si>
+    <t>Kadane's Algorithm</t>
   </si>
 </sst>
 </file>
@@ -850,14 +865,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="C79" sqref="C79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="2"/>
-    <col min="2" max="2" width="14.88671875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" style="2" customWidth="1"/>
     <col min="3" max="3" width="55.77734375" style="2" customWidth="1"/>
     <col min="4" max="4" width="9.44140625" style="2" customWidth="1"/>
     <col min="5" max="5" width="8.5546875" style="2" customWidth="1"/>
@@ -2962,15 +2977,87 @@
       <c r="A76" s="2">
         <v>75</v>
       </c>
+      <c r="B76" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F76" s="3">
+        <v>45917</v>
+      </c>
+      <c r="G76" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H76" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I76" s="2" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" s="2">
         <v>76</v>
       </c>
+      <c r="B77" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F77" s="3">
+        <v>45917</v>
+      </c>
+      <c r="G77" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H77" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I77" s="2" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" s="2">
         <v>77</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F78" s="3">
+        <v>45917</v>
+      </c>
+      <c r="G78" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H78" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I78" s="2" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved Problems: Swap Nodes in Pairs, Remove Duplicates from Sorted Linked List I, Remove Duplicates from Sorted Linked List II, Partition List & Linked List Cycle.
</commit_message>
<xml_diff>
--- a/LeetCode_Practice_Tracker_Aviral.xlsx
+++ b/LeetCode_Practice_Tracker_Aviral.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Aviral\DSAInterviewPrep\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACBA08B6-B53A-4C80-B0A8-675DE6CF2E07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43B3DEB5-4244-4CB1-8D7D-98F405FE6211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="96" windowWidth="19356" windowHeight="12144" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16410" windowHeight="10905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="159">
   <si>
     <t>ID</t>
   </si>
@@ -66,12 +66,6 @@
     <t>Sliding Window</t>
   </si>
   <si>
-    <t>Moore’s Voting</t>
-  </si>
-  <si>
-    <t>DNF Algorithm</t>
-  </si>
-  <si>
     <t>Array</t>
   </si>
   <si>
@@ -84,15 +78,9 @@
     <t>Queue</t>
   </si>
   <si>
-    <t>Hashing</t>
-  </si>
-  <si>
     <t>Linked List</t>
   </si>
   <si>
-    <t>Matrix</t>
-  </si>
-  <si>
     <t>Longest Substring Without Repeating Characters</t>
   </si>
   <si>
@@ -108,9 +96,6 @@
     <t>Sort Colors</t>
   </si>
   <si>
-    <t>Segregate 0s, 1s, and 2s</t>
-  </si>
-  <si>
     <t>Valid Anagram</t>
   </si>
   <si>
@@ -120,12 +105,6 @@
     <t>Implement Queue using Stacks</t>
   </si>
   <si>
-    <t>Two Sum II - Input array is sorted</t>
-  </si>
-  <si>
-    <t>Reverse Linked List</t>
-  </si>
-  <si>
     <t>Spiral Matrix</t>
   </si>
   <si>
@@ -490,6 +469,45 @@
   </si>
   <si>
     <t>Kadane's Algorithm</t>
+  </si>
+  <si>
+    <t>Add Two Numbers</t>
+  </si>
+  <si>
+    <t>Remove Nth node from end of Linked List</t>
+  </si>
+  <si>
+    <t>Merge 2 Sorted Linked List</t>
+  </si>
+  <si>
+    <t>Maths</t>
+  </si>
+  <si>
+    <t>Slow &amp; Fast Pointers</t>
+  </si>
+  <si>
+    <t>Merging</t>
+  </si>
+  <si>
+    <t>Swap Nodes in Pairs</t>
+  </si>
+  <si>
+    <t>Remove Duplicates from Sorted Linked List I</t>
+  </si>
+  <si>
+    <t>Remove Duplicates from Sorted Linked List II</t>
+  </si>
+  <si>
+    <t>Traversing</t>
+  </si>
+  <si>
+    <t>Partition List</t>
+  </si>
+  <si>
+    <t>2 Linked List</t>
+  </si>
+  <si>
+    <t>Linked List Cycle</t>
   </si>
 </sst>
 </file>
@@ -863,29 +881,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L94"/>
+  <dimension ref="A1:L95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="C79" sqref="C79"/>
+    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="B87" sqref="B87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="2"/>
-    <col min="2" max="2" width="15.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="55.77734375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="9.44140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="8.5546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="16.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="2"/>
+    <col min="2" max="2" width="15.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="55.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" style="2" customWidth="1"/>
     <col min="9" max="9" width="21" style="2" customWidth="1"/>
-    <col min="10" max="10" width="17.77734375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="23.88671875" style="2" customWidth="1"/>
-    <col min="12" max="12" width="8.88671875" style="2"/>
+    <col min="10" max="10" width="17.7109375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="23.85546875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -914,1315 +932,1315 @@
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F2" s="3">
         <v>45861</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="J2" s="3">
         <v>45894</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F3" s="3">
         <v>45861</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="J3" s="3">
         <v>45894</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F4" s="3">
         <v>45863</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F5" s="3">
         <v>45863</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="J6" s="3">
         <v>45894</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="J7" s="3">
         <v>45891</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="J8" s="3">
         <v>45891</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="J9" s="3">
         <v>45891</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="J10" s="3">
         <v>45891</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="J11" s="3">
         <v>45891</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="J14" s="3">
         <v>45891</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="J15" s="3">
         <v>45891</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="J16" s="3">
         <v>45894</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="J17" s="3">
         <v>45894</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="J18" s="3">
         <v>45894</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="J19" s="3">
         <v>45891</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="J20" s="3">
         <v>45891</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="J21" s="3">
         <v>45891</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="J22" s="3">
         <v>45894</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="J23" s="3">
         <v>45894</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="J24" s="3">
         <v>45891</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="J25" s="3">
         <v>45894</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="J26" s="3">
         <v>45894</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="J27" s="3">
         <v>45891</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="J29" s="3">
         <v>45894</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="J30" s="3">
         <v>45894</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="J31" s="3">
         <v>45894</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="J32" s="3">
         <v>45894</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="J33" s="3">
         <v>45891</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="J35" s="3">
         <v>45894</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C37" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>80</v>
-      </c>
       <c r="E37" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="J37" s="3">
         <v>45894</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="J39" s="3">
         <v>45894</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="J40" s="3">
         <v>45894</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="J42" s="3">
         <v>45894</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F43" s="3">
         <v>45882</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="J43" s="3">
         <v>45894</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F44" s="3">
         <v>45882</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="J44" s="3">
         <v>45891</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F45" s="3">
         <v>45887</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="J45" s="3">
         <v>45894</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F46" s="3">
         <v>45887</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="J46" s="3">
         <v>45894</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>46</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F47" s="3">
         <v>45889</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="J47" s="3">
         <v>45894</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F48" s="3">
         <v>45889</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="J48" s="3">
         <v>45894</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>48</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F49" s="3">
         <v>45889</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="J49" s="3">
         <v>45894</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -2230,28 +2248,28 @@
         <v>10</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F50" s="3">
         <v>45896</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I50" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -2259,28 +2277,28 @@
         <v>10</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F51" s="3">
         <v>45896</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I51" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -2288,28 +2306,28 @@
         <v>10</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F52" s="3">
         <v>45896</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I52" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -2317,28 +2335,28 @@
         <v>10</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F53" s="3">
         <v>45896</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -2346,28 +2364,28 @@
         <v>10</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F54" s="3">
         <v>45896</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -2375,28 +2393,28 @@
         <v>10</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F55" s="3">
         <v>45898</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I55" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -2404,28 +2422,28 @@
         <v>10</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F56" s="3">
         <v>45898</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I56" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -2433,28 +2451,28 @@
         <v>10</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F57" s="3">
         <v>45898</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I57" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -2462,28 +2480,28 @@
         <v>10</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F58" s="3">
         <v>45899</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -2491,28 +2509,28 @@
         <v>10</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F59" s="3">
         <v>45899</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -2520,28 +2538,28 @@
         <v>10</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F60" s="3">
         <v>45899</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I60" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -2549,28 +2567,28 @@
         <v>10</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F61" s="3">
         <v>45901</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I61" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>61</v>
       </c>
@@ -2578,28 +2596,28 @@
         <v>10</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F62" s="3">
         <v>45901</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I62" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>62</v>
       </c>
@@ -2607,28 +2625,28 @@
         <v>10</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F63" s="3">
         <v>45902</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I63" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>63</v>
       </c>
@@ -2636,315 +2654,315 @@
         <v>10</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F64" s="3">
         <v>45903</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I64" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>64</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F65" s="3">
         <v>45903</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I65" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>65</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F66" s="3">
         <v>45910</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I66" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>66</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F67" s="3">
         <v>45910</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I67" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>67</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F68" s="3">
         <v>45910</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I68" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>68</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I69" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>69</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F70" s="3">
         <v>45912</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I70" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>70</v>
       </c>
       <c r="B71" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C71" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C71" s="2" t="s">
-        <v>142</v>
-      </c>
       <c r="D71" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F71" s="3">
         <v>45912</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I71" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>71</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F72" s="3">
         <v>45912</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="I72" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>72</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F73" s="3">
         <v>45912</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="H73" s="2" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="I73" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>73</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F74" s="3">
         <v>45914</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H74" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I74" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>74</v>
       </c>
@@ -2952,258 +2970,411 @@
         <v>10</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F75" s="3">
         <v>45914</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H75" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I75" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>75</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F76" s="3">
         <v>45917</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H76" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I76" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>76</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F77" s="3">
         <v>45917</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H77" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I77" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>77</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F78" s="3">
         <v>45917</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I78" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>78</v>
       </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B79" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F79" s="3">
+        <v>45917</v>
+      </c>
+      <c r="G79" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H79" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I79" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>79</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B80" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F80" s="3">
+        <v>45917</v>
+      </c>
+      <c r="G80" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H80" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I80" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>80</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B81" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F81" s="3">
+        <v>45917</v>
+      </c>
+      <c r="G81" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H81" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I81" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F82" s="3">
+        <v>45919</v>
+      </c>
+      <c r="G82" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H82" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I82" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83" s="2">
+        <v>82</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F83" s="3">
+        <v>45919</v>
+      </c>
+      <c r="G83" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H83" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I83" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84" s="2">
+        <v>83</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F84" s="3">
+        <v>45919</v>
+      </c>
+      <c r="G84" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H84" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I84" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85" s="2">
+        <v>84</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F85" s="3">
+        <v>45919</v>
+      </c>
+      <c r="G85" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H85" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I85" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86" s="2">
+        <v>85</v>
+      </c>
       <c r="B86" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C86" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F86" s="3">
+        <v>45919</v>
+      </c>
+      <c r="G86" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H86" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I86" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87" s="2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88" s="2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89" s="2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A90" s="2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A91" s="2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B93" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B94" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C94" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D86" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E86" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B87" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C87" s="2" t="s">
+      <c r="D94" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B95" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C95" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D87" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E87" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B88" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C88" s="2" t="s">
+      <c r="D95" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D88" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E88" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B89" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D89" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E89" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B90" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C90" s="2" t="s">
+      <c r="E95" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="D90" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E90" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B91" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C91" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D91" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E91" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B92" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D92" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E92" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B93" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D93" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E93" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B94" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C94" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D94" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E94" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Solved Problems: Linked List Cycle II, Intersection of 2 Linked List, Remove Linked List Elements & Delete Node in a Linked List.
</commit_message>
<xml_diff>
--- a/LeetCode_Practice_Tracker_Aviral.xlsx
+++ b/LeetCode_Practice_Tracker_Aviral.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Aviral\DSAInterviewPrep\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43B3DEB5-4244-4CB1-8D7D-98F405FE6211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9E53532-2068-4CB8-80EB-6EFBEB627EDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16410" windowHeight="10905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="105" windowWidth="16410" windowHeight="10425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="163">
   <si>
     <t>ID</t>
   </si>
@@ -508,6 +508,18 @@
   </si>
   <si>
     <t>Linked List Cycle</t>
+  </si>
+  <si>
+    <t>Linked List Cycle II</t>
+  </si>
+  <si>
+    <t>Intersection of 2 Linked List</t>
+  </si>
+  <si>
+    <t>Remove Linked List Elements</t>
+  </si>
+  <si>
+    <t>Delete Node in a Linked List</t>
   </si>
 </sst>
 </file>
@@ -884,7 +896,7 @@
   <dimension ref="A1:L95"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="B87" sqref="B87"/>
+      <selection activeCell="B91" sqref="B91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3314,20 +3326,107 @@
       <c r="A87" s="2">
         <v>86</v>
       </c>
+      <c r="B87" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F87" s="3">
+        <v>45919</v>
+      </c>
+      <c r="G87" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H87" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I87" s="2" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>87</v>
       </c>
+      <c r="B88" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F88" s="3">
+        <v>45919</v>
+      </c>
+      <c r="G88" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="H88" s="2" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>88</v>
       </c>
+      <c r="B89" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F89" s="3">
+        <v>45919</v>
+      </c>
+      <c r="G89" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H89" s="2" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>89</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F90" s="3">
+        <v>45919</v>
+      </c>
+      <c r="G90" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H90" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Solved Problems: Reverse Linked List, Reverse Linked List II, Odd Even Linked List and Linked List Random Pointer.
</commit_message>
<xml_diff>
--- a/LeetCode_Practice_Tracker_Aviral.xlsx
+++ b/LeetCode_Practice_Tracker_Aviral.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Aviral\DSAInterviewPrep\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9E53532-2068-4CB8-80EB-6EFBEB627EDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B0DE4A-0E40-4703-80B3-454558D7DF7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="105" windowWidth="16410" windowHeight="10425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="169">
   <si>
     <t>ID</t>
   </si>
@@ -520,6 +520,24 @@
   </si>
   <si>
     <t>Delete Node in a Linked List</t>
+  </si>
+  <si>
+    <t>Reverse Linked List</t>
+  </si>
+  <si>
+    <t>Swapping next pointer</t>
+  </si>
+  <si>
+    <t>Reverse Linked List II</t>
+  </si>
+  <si>
+    <t>Odd &amp; Even Linked List</t>
+  </si>
+  <si>
+    <t>Linked List Random Nodw</t>
+  </si>
+  <si>
+    <t>Using Random Class</t>
   </si>
 </sst>
 </file>
@@ -893,10 +911,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L95"/>
+  <dimension ref="A1:L112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="B91" sqref="B91"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="A95" sqref="A95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3433,46 +3451,192 @@
       <c r="A91" s="2">
         <v>90</v>
       </c>
+      <c r="B91" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F91" s="3">
+        <v>45922</v>
+      </c>
+      <c r="G91" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H91" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I91" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A92" s="2">
+        <v>91</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F92" s="3">
+        <v>45922</v>
+      </c>
+      <c r="G92" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H92" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I92" s="2" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A93" s="2">
+        <v>92</v>
+      </c>
       <c r="B93" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F93" s="3">
+        <v>45922</v>
+      </c>
+      <c r="G93" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H93" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I93" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A94" s="2">
+        <v>93</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F94" s="3">
+        <v>45922</v>
+      </c>
+      <c r="G94" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H94" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I94" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A95" s="2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A96" s="2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" s="2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" s="2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" s="2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" s="2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B110" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C93" s="2" t="s">
+      <c r="C110" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D93" s="2" t="s">
+      <c r="D110" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E93" s="2" t="s">
+      <c r="E110" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B94" s="2" t="s">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B111" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C94" s="2" t="s">
+      <c r="C111" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D94" s="2" t="s">
+      <c r="D111" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E94" s="2" t="s">
+      <c r="E111" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B95" s="2" t="s">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B112" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C95" s="2" t="s">
+      <c r="C112" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D95" s="2" t="s">
+      <c r="D112" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E95" s="2" t="s">
+      <c r="E112" s="2" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Solved Problems: Middle of Linked List, Next Greater Node in Linked List, Merge in Between Linked List & Swapping Nodes in a Linked List.
</commit_message>
<xml_diff>
--- a/LeetCode_Practice_Tracker_Aviral.xlsx
+++ b/LeetCode_Practice_Tracker_Aviral.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Aviral\DSAInterviewPrep\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B0DE4A-0E40-4703-80B3-454558D7DF7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC7EFB1B-8E0D-4794-9FCF-6566087750B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="105" windowWidth="16410" windowHeight="10425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="174">
   <si>
     <t>ID</t>
   </si>
@@ -538,6 +538,21 @@
   </si>
   <si>
     <t>Using Random Class</t>
+  </si>
+  <si>
+    <t>Middle Of Linked List</t>
+  </si>
+  <si>
+    <t>Next Greater Element Node in Linked List</t>
+  </si>
+  <si>
+    <t>Using Stack</t>
+  </si>
+  <si>
+    <t>Merge in Between Linked List</t>
+  </si>
+  <si>
+    <t>Swapping Nodes in a Linked List</t>
   </si>
 </sst>
 </file>
@@ -914,7 +929,7 @@
   <dimension ref="A1:L112"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="A95" sqref="A95"/>
+      <selection activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3567,38 +3582,128 @@
       <c r="A95" s="2">
         <v>94</v>
       </c>
+      <c r="B95" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F95" s="3">
+        <v>45924</v>
+      </c>
+      <c r="G95" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H95" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I95" s="2" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>95</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B96" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F96" s="3">
+        <v>45924</v>
+      </c>
+      <c r="G96" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H96" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I96" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>96</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B97" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F97" s="3">
+        <v>45924</v>
+      </c>
+      <c r="G97" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H97" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>97</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B98" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F98" s="3">
+        <v>45924</v>
+      </c>
+      <c r="G98" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H98" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>100</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B110" s="2" t="s">
         <v>12</v>
       </c>
@@ -3612,7 +3717,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B111" s="2" t="s">
         <v>13</v>
       </c>
@@ -3626,7 +3731,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B112" s="2" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Solved Problems: LRU Cache.
</commit_message>
<xml_diff>
--- a/LeetCode_Practice_Tracker_Aviral.xlsx
+++ b/LeetCode_Practice_Tracker_Aviral.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Aviral\DSAInterviewPrep\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC7EFB1B-8E0D-4794-9FCF-6566087750B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0AD697B-0C87-43E0-9329-E7D5710822D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="105" windowWidth="16410" windowHeight="10425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16410" windowHeight="10905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="177">
   <si>
     <t>ID</t>
   </si>
@@ -553,6 +553,15 @@
   </si>
   <si>
     <t>Swapping Nodes in a Linked List</t>
+  </si>
+  <si>
+    <t>LRU Cache</t>
+  </si>
+  <si>
+    <t>O(Capacity)</t>
+  </si>
+  <si>
+    <t>Using HashMap</t>
   </si>
 </sst>
 </file>
@@ -929,7 +938,7 @@
   <dimension ref="A1:L112"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="C88" sqref="C88"/>
+      <selection activeCell="I100" sqref="I100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3636,7 +3645,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>96</v>
       </c>
@@ -3662,7 +3671,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>97</v>
       </c>
@@ -3688,22 +3697,46 @@
         <v>33</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <v>98</v>
       </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B99" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F99" s="3">
+        <v>45924</v>
+      </c>
+      <c r="G99" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H99" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="I99" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>100</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B110" s="2" t="s">
         <v>12</v>
       </c>
@@ -3717,7 +3750,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B111" s="2" t="s">
         <v>13</v>
       </c>
@@ -3731,7 +3764,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B112" s="2" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Solved Problems: Reverse Nodes in K group, Rotate List, Insertion Sort and Design Linked List.
</commit_message>
<xml_diff>
--- a/LeetCode_Practice_Tracker_Aviral.xlsx
+++ b/LeetCode_Practice_Tracker_Aviral.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Aviral\DSAInterviewPrep\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0AD697B-0C87-43E0-9329-E7D5710822D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57A538C2-A54D-43C5-8E0D-8AB985919ECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16410" windowHeight="10905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="105" windowWidth="16410" windowHeight="10425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="182">
   <si>
     <t>ID</t>
   </si>
@@ -562,6 +562,21 @@
   </si>
   <si>
     <t>Using HashMap</t>
+  </si>
+  <si>
+    <t>Reverse Nodes in K Group</t>
+  </si>
+  <si>
+    <t>Rotate List</t>
+  </si>
+  <si>
+    <t>Insertion Sort</t>
+  </si>
+  <si>
+    <t>o(n ^ 2)</t>
+  </si>
+  <si>
+    <t>Design Linked List</t>
   </si>
 </sst>
 </file>
@@ -937,8 +952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="I100" sqref="I100"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="A107" sqref="A107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3730,13 +3745,146 @@
       <c r="A100" s="2">
         <v>99</v>
       </c>
+      <c r="B100" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F100" s="3">
+        <v>45925</v>
+      </c>
+      <c r="G100" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H100" s="2" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>100</v>
       </c>
+      <c r="B101" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F101" s="3">
+        <v>45925</v>
+      </c>
+      <c r="G101" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H101" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I101" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A102" s="2">
+        <v>101</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F102" s="3">
+        <v>45925</v>
+      </c>
+      <c r="G102" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="H102" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I102" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A103" s="2">
+        <v>102</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F103" s="3">
+        <v>45925</v>
+      </c>
+      <c r="G103" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H103" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A104" s="2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A105" s="2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A106" s="2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A107" s="2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A108" s="2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A109" s="2">
+        <v>108</v>
+      </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A110" s="2">
+        <v>109</v>
+      </c>
       <c r="B110" s="2" t="s">
         <v>12</v>
       </c>
@@ -3751,6 +3899,9 @@
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A111" s="2">
+        <v>110</v>
+      </c>
       <c r="B111" s="2" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
Solved Problems: Clone Linked List with Random Pointer, Palindrome Linked List & Merge Sort.
</commit_message>
<xml_diff>
--- a/LeetCode_Practice_Tracker_Aviral.xlsx
+++ b/LeetCode_Practice_Tracker_Aviral.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Aviral\DSAInterviewPrep\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57A538C2-A54D-43C5-8E0D-8AB985919ECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0040C66A-8247-4CFA-B405-1458C26090CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="105" windowWidth="16410" windowHeight="10425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="185">
   <si>
     <t>ID</t>
   </si>
@@ -577,6 +577,15 @@
   </si>
   <si>
     <t>Design Linked List</t>
+  </si>
+  <si>
+    <t>Clone Linked List with Random Pointer</t>
+  </si>
+  <si>
+    <t>Palindrom Linked List</t>
+  </si>
+  <si>
+    <t>Reversing</t>
   </si>
 </sst>
 </file>
@@ -953,7 +962,7 @@
   <dimension ref="A1:L112"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="A107" sqref="A107"/>
+      <selection activeCell="B107" sqref="B107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3855,15 +3864,84 @@
       <c r="A104" s="2">
         <v>103</v>
       </c>
+      <c r="B104" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F104" s="3">
+        <v>45926</v>
+      </c>
+      <c r="G104" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H104" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I104" s="2" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <v>104</v>
       </c>
+      <c r="B105" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E105" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F105" s="3">
+        <v>45926</v>
+      </c>
+      <c r="G105" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H105" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I105" s="2" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
         <v>105</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E106" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F106" s="3">
+        <v>45926</v>
+      </c>
+      <c r="G106" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="H106" s="2" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Solved Problems: Reorder List & Flatten a multilevel doubly linked list.
</commit_message>
<xml_diff>
--- a/LeetCode_Practice_Tracker_Aviral.xlsx
+++ b/LeetCode_Practice_Tracker_Aviral.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Aviral\DSAInterviewPrep\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0040C66A-8247-4CFA-B405-1458C26090CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{243AFA6C-E298-4B5B-829A-B1E1B1E1FA88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="105" windowWidth="16410" windowHeight="10425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="189">
   <si>
     <t>ID</t>
   </si>
@@ -586,6 +586,18 @@
   </si>
   <si>
     <t>Reversing</t>
+  </si>
+  <si>
+    <t>Reorder List</t>
+  </si>
+  <si>
+    <t>Reverse &amp; Merge</t>
+  </si>
+  <si>
+    <t>Flatten a Doubly Linked List</t>
+  </si>
+  <si>
+    <t>DFS</t>
   </si>
 </sst>
 </file>
@@ -962,7 +974,7 @@
   <dimension ref="A1:L112"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="B107" sqref="B107"/>
+      <selection activeCell="A109" sqref="A109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3948,10 +3960,58 @@
       <c r="A107" s="2">
         <v>106</v>
       </c>
+      <c r="B107" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E107" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F107" s="3">
+        <v>45929</v>
+      </c>
+      <c r="G107" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H107" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I107" s="2" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
         <v>107</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E108" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F108" s="3">
+        <v>45929</v>
+      </c>
+      <c r="G108" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H108" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I108" s="2" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Solved Problems: 1. Valid Parentheses 2. Min Stack 3. Simplify Stack
</commit_message>
<xml_diff>
--- a/LeetCode_Practice_Tracker_Aviral.xlsx
+++ b/LeetCode_Practice_Tracker_Aviral.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Aviral\DSAInterviewPrep\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{243AFA6C-E298-4B5B-829A-B1E1B1E1FA88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09AF14FC-9CA4-464D-82DC-A929029602FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="105" windowWidth="16410" windowHeight="10425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="203">
   <si>
     <t>ID</t>
   </si>
@@ -598,6 +598,48 @@
   </si>
   <si>
     <t>DFS</t>
+  </si>
+  <si>
+    <t>Min Stack</t>
+  </si>
+  <si>
+    <t>Implement Stack using Array / Linked List</t>
+  </si>
+  <si>
+    <t>Implement Stack using Queues</t>
+  </si>
+  <si>
+    <t>Next Greater Element I</t>
+  </si>
+  <si>
+    <t>Next Greater Element II (Circular)</t>
+  </si>
+  <si>
+    <t>Daily Temperatures</t>
+  </si>
+  <si>
+    <t>Evaluate Reverse Polish Notation</t>
+  </si>
+  <si>
+    <t>Largest Rectangle in Histogram</t>
+  </si>
+  <si>
+    <t>Trapping Rain Water (Stack approach)</t>
+  </si>
+  <si>
+    <t>Remove K Digits</t>
+  </si>
+  <si>
+    <t>Decode String</t>
+  </si>
+  <si>
+    <t>Asteroid Collision</t>
+  </si>
+  <si>
+    <t>Online Stock Span</t>
+  </si>
+  <si>
+    <t>Simplify Path</t>
   </si>
 </sst>
 </file>
@@ -971,29 +1013,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L112"/>
+  <dimension ref="A1:L130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="A109" sqref="A109"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="I123" sqref="I123"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="2"/>
-    <col min="2" max="2" width="15.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="55.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="2"/>
+    <col min="2" max="2" width="15.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="55.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="9.44140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="8.5546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" style="2" customWidth="1"/>
     <col min="9" max="9" width="21" style="2" customWidth="1"/>
-    <col min="10" max="10" width="17.7109375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="23.85546875" style="2" customWidth="1"/>
-    <col min="12" max="12" width="8.85546875" style="2"/>
+    <col min="10" max="10" width="17.6640625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="23.88671875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1028,7 +1070,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1060,7 +1102,7 @@
         <v>45894</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1092,7 +1134,7 @@
         <v>45894</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1121,7 +1163,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1150,7 +1192,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1179,7 +1221,7 @@
         <v>45894</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1205,7 +1247,7 @@
         <v>45891</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1231,7 +1273,7 @@
         <v>45891</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1260,7 +1302,7 @@
         <v>45891</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1289,7 +1331,7 @@
         <v>45891</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1318,7 +1360,7 @@
         <v>45891</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1332,7 +1374,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1346,7 +1388,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1372,7 +1414,7 @@
         <v>45891</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1401,7 +1443,7 @@
         <v>45891</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1427,7 +1469,7 @@
         <v>45894</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1456,7 +1498,7 @@
         <v>45894</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1485,7 +1527,7 @@
         <v>45894</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1514,7 +1556,7 @@
         <v>45891</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1543,7 +1585,7 @@
         <v>45891</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1569,7 +1611,7 @@
         <v>45891</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1595,7 +1637,7 @@
         <v>45894</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -1624,7 +1666,7 @@
         <v>45894</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -1653,7 +1695,7 @@
         <v>45891</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -1682,7 +1724,7 @@
         <v>45894</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -1711,7 +1753,7 @@
         <v>45894</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -1737,7 +1779,7 @@
         <v>45891</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -1751,7 +1793,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -1780,7 +1822,7 @@
         <v>45894</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -1809,7 +1851,7 @@
         <v>45894</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -1838,7 +1880,7 @@
         <v>45894</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -1867,7 +1909,7 @@
         <v>45894</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -1893,7 +1935,7 @@
         <v>45891</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -1907,7 +1949,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -1936,7 +1978,7 @@
         <v>45894</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -1950,7 +1992,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -1982,7 +2024,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -2008,7 +2050,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -2037,7 +2079,7 @@
         <v>45894</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -2066,7 +2108,7 @@
         <v>45894</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -2080,7 +2122,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -2106,7 +2148,7 @@
         <v>45894</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -2138,7 +2180,7 @@
         <v>45894</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -2170,7 +2212,7 @@
         <v>45891</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -2202,7 +2244,7 @@
         <v>45894</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -2234,7 +2276,7 @@
         <v>45894</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -2266,7 +2308,7 @@
         <v>45894</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -2298,7 +2340,7 @@
         <v>45894</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -2330,7 +2372,7 @@
         <v>45894</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -2359,7 +2401,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -2388,7 +2430,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -2417,7 +2459,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -2446,7 +2488,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -2475,7 +2517,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -2504,7 +2546,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -2533,7 +2575,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -2562,7 +2604,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -2591,7 +2633,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -2620,7 +2662,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -2649,7 +2691,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -2678,7 +2720,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <v>61</v>
       </c>
@@ -2707,7 +2749,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
         <v>62</v>
       </c>
@@ -2736,7 +2778,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
         <v>63</v>
       </c>
@@ -2765,7 +2807,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -2794,7 +2836,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
         <v>65</v>
       </c>
@@ -2823,7 +2865,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
         <v>66</v>
       </c>
@@ -2852,7 +2894,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
         <v>67</v>
       </c>
@@ -2881,7 +2923,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" s="2">
         <v>68</v>
       </c>
@@ -2907,7 +2949,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" s="2">
         <v>69</v>
       </c>
@@ -2936,7 +2978,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" s="2">
         <v>70</v>
       </c>
@@ -2965,7 +3007,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" s="2">
         <v>71</v>
       </c>
@@ -2994,7 +3036,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" s="2">
         <v>72</v>
       </c>
@@ -3023,7 +3065,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="2">
         <v>73</v>
       </c>
@@ -3052,7 +3094,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" s="2">
         <v>74</v>
       </c>
@@ -3081,7 +3123,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" s="2">
         <v>75</v>
       </c>
@@ -3110,7 +3152,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" s="2">
         <v>76</v>
       </c>
@@ -3139,7 +3181,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" s="2">
         <v>77</v>
       </c>
@@ -3168,7 +3210,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" s="2">
         <v>78</v>
       </c>
@@ -3197,7 +3239,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" s="2">
         <v>79</v>
       </c>
@@ -3226,7 +3268,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" s="2">
         <v>80</v>
       </c>
@@ -3255,7 +3297,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" s="2">
         <v>81</v>
       </c>
@@ -3284,7 +3326,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" s="2">
         <v>82</v>
       </c>
@@ -3313,7 +3355,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" s="2">
         <v>83</v>
       </c>
@@ -3342,7 +3384,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" s="2">
         <v>84</v>
       </c>
@@ -3371,7 +3413,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" s="2">
         <v>85</v>
       </c>
@@ -3400,7 +3442,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" s="2">
         <v>86</v>
       </c>
@@ -3429,7 +3471,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" s="2">
         <v>87</v>
       </c>
@@ -3455,7 +3497,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" s="2">
         <v>88</v>
       </c>
@@ -3481,7 +3523,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" s="2">
         <v>89</v>
       </c>
@@ -3507,7 +3549,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" s="2">
         <v>90</v>
       </c>
@@ -3536,7 +3578,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" s="2">
         <v>91</v>
       </c>
@@ -3565,7 +3607,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" s="2">
         <v>92</v>
       </c>
@@ -3594,7 +3636,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" s="2">
         <v>93</v>
       </c>
@@ -3623,7 +3665,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" s="2">
         <v>94</v>
       </c>
@@ -3652,7 +3694,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" s="2">
         <v>95</v>
       </c>
@@ -3681,7 +3723,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97" s="2">
         <v>96</v>
       </c>
@@ -3707,7 +3749,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" s="2">
         <v>97</v>
       </c>
@@ -3733,7 +3775,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" s="2">
         <v>98</v>
       </c>
@@ -3762,7 +3804,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" s="2">
         <v>99</v>
       </c>
@@ -3788,7 +3830,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" s="2">
         <v>100</v>
       </c>
@@ -3817,7 +3859,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102" s="2">
         <v>101</v>
       </c>
@@ -3846,7 +3888,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103" s="2">
         <v>102</v>
       </c>
@@ -3872,7 +3914,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104" s="2">
         <v>103</v>
       </c>
@@ -3901,7 +3943,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A105" s="2">
         <v>104</v>
       </c>
@@ -3930,7 +3972,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A106" s="2">
         <v>105</v>
       </c>
@@ -3956,7 +3998,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A107" s="2">
         <v>106</v>
       </c>
@@ -3985,7 +4027,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A108" s="2">
         <v>107</v>
       </c>
@@ -4014,29 +4056,59 @@
         <v>188</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A109" s="2">
         <v>108</v>
       </c>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B109" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D109" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E109" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F109" s="3">
+        <v>45662</v>
+      </c>
+      <c r="G109" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H109" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A110" s="2">
         <v>109</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>21</v>
+        <v>189</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="F110" s="3">
+        <v>45662</v>
+      </c>
+      <c r="G110" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H110" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A111" s="2">
         <v>110</v>
       </c>
@@ -4044,27 +4116,225 @@
         <v>13</v>
       </c>
       <c r="C111" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A112" s="2">
+        <v>111</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A113" s="2">
+        <v>112</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A114" s="2">
+        <v>113</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A115" s="2">
+        <v>114</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A116" s="2">
+        <v>115</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A117" s="2">
+        <v>116</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A118" s="2">
+        <v>117</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A119" s="2">
+        <v>118</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A120" s="2">
+        <v>119</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A121" s="2">
+        <v>120</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A122" s="2">
+        <v>121</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A123" s="2">
+        <v>123</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D123" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E123" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F123" s="3">
+        <v>45662</v>
+      </c>
+      <c r="G123" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H123" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A124" s="2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A125" s="2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A126" s="2">
+        <v>126</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D126" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E126" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A127" s="2">
+        <v>127</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C127" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D111" s="2" t="s">
+      <c r="D127" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E111" s="2" t="s">
+      <c r="E127" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B112" s="2" t="s">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A128" s="2">
+        <v>128</v>
+      </c>
+      <c r="B128" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C112" s="2" t="s">
+      <c r="C128" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D112" s="2" t="s">
+      <c r="D128" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E112" s="2" t="s">
+      <c r="E128" s="2" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A129" s="2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A130" s="2">
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Solved Problems: 1. Next Greater Element I 2. Next Greater Element II
</commit_message>
<xml_diff>
--- a/LeetCode_Practice_Tracker_Aviral.xlsx
+++ b/LeetCode_Practice_Tracker_Aviral.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Aviral\DSAInterviewPrep\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09AF14FC-9CA4-464D-82DC-A929029602FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3839769-07F5-4580-ACEB-64F8C4235715}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="204">
   <si>
     <t>ID</t>
   </si>
@@ -640,6 +640,9 @@
   </si>
   <si>
     <t>Simplify Path</t>
+  </si>
+  <si>
+    <t>Monotonic Stack</t>
   </si>
 </sst>
 </file>
@@ -1016,7 +1019,7 @@
   <dimension ref="A1:L130"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="I123" sqref="I123"/>
+      <selection activeCell="I114" sqref="I114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4130,7 +4133,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A113" s="2">
         <v>112</v>
       </c>
@@ -4140,8 +4143,26 @@
       <c r="C113" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D113" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E113" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F113" s="3">
+        <v>45664</v>
+      </c>
+      <c r="G113" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="H113" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I113" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A114" s="2">
         <v>113</v>
       </c>
@@ -4151,8 +4172,26 @@
       <c r="C114" s="2" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D114" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E114" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F114" s="3">
+        <v>45664</v>
+      </c>
+      <c r="G114" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H114" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I114" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A115" s="2">
         <v>114</v>
       </c>
@@ -4163,7 +4202,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A116" s="2">
         <v>115</v>
       </c>
@@ -4174,7 +4213,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A117" s="2">
         <v>116</v>
       </c>
@@ -4185,7 +4224,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A118" s="2">
         <v>117</v>
       </c>
@@ -4196,7 +4235,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A119" s="2">
         <v>118</v>
       </c>
@@ -4207,7 +4246,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A120" s="2">
         <v>119</v>
       </c>
@@ -4218,7 +4257,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A121" s="2">
         <v>120</v>
       </c>
@@ -4229,7 +4268,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A122" s="2">
         <v>121</v>
       </c>
@@ -4240,7 +4279,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A123" s="2">
         <v>123</v>
       </c>
@@ -4266,17 +4305,17 @@
         <v>30</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A124" s="2">
         <v>124</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A125" s="2">
         <v>125</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A126" s="2">
         <v>126</v>
       </c>
@@ -4293,7 +4332,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A127" s="2">
         <v>127</v>
       </c>
@@ -4310,7 +4349,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A128" s="2">
         <v>128</v>
       </c>

</xml_diff>

<commit_message>
Solved Problems: 1. Daily Temperatures. 2. Evaluate Reverse Polish Notations.
</commit_message>
<xml_diff>
--- a/LeetCode_Practice_Tracker_Aviral.xlsx
+++ b/LeetCode_Practice_Tracker_Aviral.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Aviral\DSAInterviewPrep\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3839769-07F5-4580-ACEB-64F8C4235715}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88E9929D-8475-46D8-80AA-714465040CE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="204">
   <si>
     <t>ID</t>
   </si>
@@ -1018,8 +1018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="I114" sqref="I114"/>
+    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="I116" sqref="I116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4201,6 +4201,24 @@
       <c r="C115" s="2" t="s">
         <v>194</v>
       </c>
+      <c r="D115" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E115" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F115" s="3">
+        <v>45664</v>
+      </c>
+      <c r="G115" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H115" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I115" s="2" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A116" s="2">
@@ -4211,6 +4229,21 @@
       </c>
       <c r="C116" s="2" t="s">
         <v>195</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E116" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F116" s="3">
+        <v>45664</v>
+      </c>
+      <c r="G116" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H116" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved Problems: 1. Asteroid Collision. 2. Online Stock Span.
</commit_message>
<xml_diff>
--- a/LeetCode_Practice_Tracker_Aviral.xlsx
+++ b/LeetCode_Practice_Tracker_Aviral.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Aviral\DSAInterviewPrep\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88E9929D-8475-46D8-80AA-714465040CE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9444C44-6DD7-4149-B7F6-F390D2D22F06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="204">
   <si>
     <t>ID</t>
   </si>
@@ -1019,7 +1019,7 @@
   <dimension ref="A1:L130"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="I116" sqref="I116"/>
+      <selection activeCell="H122" sqref="H122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4300,6 +4300,21 @@
       <c r="C121" s="2" t="s">
         <v>200</v>
       </c>
+      <c r="D121" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E121" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F121" s="3">
+        <v>45665</v>
+      </c>
+      <c r="G121" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H121" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A122" s="2">
@@ -4310,6 +4325,24 @@
       </c>
       <c r="C122" s="2" t="s">
         <v>201</v>
+      </c>
+      <c r="D122" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E122" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F122" s="3">
+        <v>45665</v>
+      </c>
+      <c r="G122" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H122" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I122" s="2" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved Problems: 1. Implementation of Stack Using Array. 2. Implementation of Stack Using Linked List. 3. Implementation of Stack Using Queues.
</commit_message>
<xml_diff>
--- a/LeetCode_Practice_Tracker_Aviral.xlsx
+++ b/LeetCode_Practice_Tracker_Aviral.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Aviral\DSAInterviewPrep\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9444C44-6DD7-4149-B7F6-F390D2D22F06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A5FB03F-4FC3-46A7-BA50-39DA3B5B2035}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="206">
   <si>
     <t>ID</t>
   </si>
@@ -603,9 +603,6 @@
     <t>Min Stack</t>
   </si>
   <si>
-    <t>Implement Stack using Array / Linked List</t>
-  </si>
-  <si>
     <t>Implement Stack using Queues</t>
   </si>
   <si>
@@ -643,6 +640,15 @@
   </si>
   <si>
     <t>Monotonic Stack</t>
+  </si>
+  <si>
+    <t>Implement Stack using Array</t>
+  </si>
+  <si>
+    <t>Implement Stack using Linked List</t>
+  </si>
+  <si>
+    <t>Push O(n) Pop O(1)</t>
   </si>
 </sst>
 </file>
@@ -1018,8 +1024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="H122" sqref="H122"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="G114" sqref="G114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1030,7 +1036,7 @@
     <col min="4" max="4" width="9.44140625" style="2" customWidth="1"/>
     <col min="5" max="5" width="8.5546875" style="2" customWidth="1"/>
     <col min="6" max="6" width="12.44140625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" style="2" customWidth="1"/>
     <col min="8" max="8" width="16.6640625" style="2" customWidth="1"/>
     <col min="9" max="9" width="21" style="2" customWidth="1"/>
     <col min="10" max="10" width="17.6640625" style="2" customWidth="1"/>
@@ -4119,7 +4125,22 @@
         <v>13</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>190</v>
+        <v>203</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E111" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F111" s="3">
+        <v>45665</v>
+      </c>
+      <c r="G111" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H111" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.3">
@@ -4130,7 +4151,22 @@
         <v>13</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>191</v>
+        <v>204</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E112" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F112" s="3">
+        <v>45665</v>
+      </c>
+      <c r="G112" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H112" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.3">
@@ -4141,7 +4177,7 @@
         <v>13</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D113" s="2" t="s">
         <v>25</v>
@@ -4150,16 +4186,13 @@
         <v>28</v>
       </c>
       <c r="F113" s="3">
-        <v>45664</v>
+        <v>45665</v>
       </c>
       <c r="G113" s="2" t="s">
-        <v>106</v>
+        <v>205</v>
       </c>
       <c r="H113" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I113" s="2" t="s">
-        <v>203</v>
+        <v>33</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.3">
@@ -4170,10 +4203,10 @@
         <v>13</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E114" s="2" t="s">
         <v>28</v>
@@ -4182,13 +4215,13 @@
         <v>45664</v>
       </c>
       <c r="G114" s="2" t="s">
-        <v>30</v>
+        <v>106</v>
       </c>
       <c r="H114" s="2" t="s">
         <v>30</v>
       </c>
       <c r="I114" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.3">
@@ -4199,7 +4232,7 @@
         <v>13</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D115" s="2" t="s">
         <v>26</v>
@@ -4217,7 +4250,7 @@
         <v>30</v>
       </c>
       <c r="I115" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.3">
@@ -4228,7 +4261,7 @@
         <v>13</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D116" s="2" t="s">
         <v>26</v>
@@ -4244,6 +4277,9 @@
       </c>
       <c r="H116" s="2" t="s">
         <v>30</v>
+      </c>
+      <c r="I116" s="2" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.3">
@@ -4254,7 +4290,22 @@
         <v>13</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
+      </c>
+      <c r="D117" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E117" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F117" s="3">
+        <v>45664</v>
+      </c>
+      <c r="G117" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H117" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.3">
@@ -4265,7 +4316,7 @@
         <v>13</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.3">
@@ -4276,7 +4327,7 @@
         <v>13</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.3">
@@ -4287,7 +4338,7 @@
         <v>13</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.3">
@@ -4298,22 +4349,7 @@
         <v>13</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="D121" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E121" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F121" s="3">
-        <v>45665</v>
-      </c>
-      <c r="G121" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H121" s="2" t="s">
-        <v>30</v>
+        <v>198</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.3">
@@ -4324,7 +4360,7 @@
         <v>13</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D122" s="2" t="s">
         <v>26</v>
@@ -4336,13 +4372,10 @@
         <v>45665</v>
       </c>
       <c r="G122" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H122" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="I122" s="2" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.3">
@@ -4353,28 +4386,52 @@
         <v>13</v>
       </c>
       <c r="C123" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="D123" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E123" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F123" s="3">
+        <v>45665</v>
+      </c>
+      <c r="G123" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H123" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I123" s="2" t="s">
         <v>202</v>
-      </c>
-      <c r="D123" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E123" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F123" s="3">
-        <v>45662</v>
-      </c>
-      <c r="G123" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H123" s="2" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A124" s="2">
         <v>124</v>
       </c>
+      <c r="B124" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="D124" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E124" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F124" s="3">
+        <v>45662</v>
+      </c>
+      <c r="G124" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H124" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A125" s="2">
@@ -4385,28 +4442,16 @@
       <c r="A126" s="2">
         <v>126</v>
       </c>
-      <c r="B126" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C126" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D126" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E126" s="2" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A127" s="2">
         <v>127</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D127" s="2" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
Solved Problems: 1. Decode String 2. Remove K Digits
</commit_message>
<xml_diff>
--- a/LeetCode_Practice_Tracker_Aviral.xlsx
+++ b/LeetCode_Practice_Tracker_Aviral.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Aviral\DSAInterviewPrep\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A5FB03F-4FC3-46A7-BA50-39DA3B5B2035}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3501733B-0BBE-4EF4-87F6-487EBF971F69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="206">
   <si>
     <t>ID</t>
   </si>
@@ -1024,8 +1024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="G114" sqref="G114"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="D120" sqref="D120:H120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4340,6 +4340,21 @@
       <c r="C120" s="2" t="s">
         <v>197</v>
       </c>
+      <c r="D120" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E120" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F120" s="3">
+        <v>45669</v>
+      </c>
+      <c r="G120" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H120" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A121" s="2">
@@ -4350,6 +4365,21 @@
       </c>
       <c r="C121" s="2" t="s">
         <v>198</v>
+      </c>
+      <c r="D121" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E121" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F121" s="3">
+        <v>45669</v>
+      </c>
+      <c r="G121" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H121" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved Problems: 1. Largest Rectangle in Histogram. 2. Trapping Rain Water (Stack Approach).
</commit_message>
<xml_diff>
--- a/LeetCode_Practice_Tracker_Aviral.xlsx
+++ b/LeetCode_Practice_Tracker_Aviral.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Aviral\DSAInterviewPrep\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3501733B-0BBE-4EF4-87F6-487EBF971F69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{802FCC42-E12F-484B-A857-9218AA9CF9F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="206">
   <si>
     <t>ID</t>
   </si>
@@ -1025,7 +1025,7 @@
   <dimension ref="A1:L130"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="D120" sqref="D120:H120"/>
+      <selection activeCell="D119" sqref="D119:I119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4318,6 +4318,24 @@
       <c r="C118" s="2" t="s">
         <v>195</v>
       </c>
+      <c r="D118" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E118" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F118" s="3">
+        <v>45670</v>
+      </c>
+      <c r="G118" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H118" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I118" s="2" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A119" s="2">
@@ -4328,6 +4346,24 @@
       </c>
       <c r="C119" s="2" t="s">
         <v>196</v>
+      </c>
+      <c r="D119" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E119" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F119" s="3">
+        <v>45670</v>
+      </c>
+      <c r="G119" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H119" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I119" s="2" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved Problems: 1. Design Circular Queue 2. Implement Queue using Stacks 3. Time Needed to But Tickets
</commit_message>
<xml_diff>
--- a/LeetCode_Practice_Tracker_Aviral.xlsx
+++ b/LeetCode_Practice_Tracker_Aviral.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Aviral\DSAInterviewPrep\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{802FCC42-E12F-484B-A857-9218AA9CF9F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4CBEA08-235F-48BE-A070-05D666BBECA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="214">
   <si>
     <t>ID</t>
   </si>
@@ -649,6 +649,30 @@
   </si>
   <si>
     <t>Push O(n) Pop O(1)</t>
+  </si>
+  <si>
+    <t>Design Circular Queue</t>
+  </si>
+  <si>
+    <t>Design Hit Counter</t>
+  </si>
+  <si>
+    <t>O(n) Amortized O(1)</t>
+  </si>
+  <si>
+    <t>Moving Average from Data Stream</t>
+  </si>
+  <si>
+    <t>Number of Recent Calls</t>
+  </si>
+  <si>
+    <t>Time Needed to Buy Tickets</t>
+  </si>
+  <si>
+    <t>Dota2 Senate</t>
+  </si>
+  <si>
+    <t>O(capacity)</t>
   </si>
 </sst>
 </file>
@@ -1022,10 +1046,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L130"/>
+  <dimension ref="A1:L142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="D119" sqref="D119:I119"/>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="C128" sqref="C128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4503,27 +4527,63 @@
       <c r="A125" s="2">
         <v>125</v>
       </c>
+      <c r="B125" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C125" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D125" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E125" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F125" s="3">
+        <v>46037</v>
+      </c>
+      <c r="G125" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="H125" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A126" s="2">
         <v>126</v>
       </c>
+      <c r="B126" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D126" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E126" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F126" s="3">
+        <v>46037</v>
+      </c>
+      <c r="G126" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H126" s="2" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A127" s="2">
         <v>127</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D127" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E127" s="2" t="s">
-        <v>27</v>
+        <v>209</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.3">
@@ -4534,23 +4594,69 @@
         <v>14</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D128" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E128" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A129" s="2">
         <v>129</v>
       </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B129" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A130" s="2">
         <v>130</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A131" s="2">
+        <v>131</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="D131" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E131" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F131" s="3">
+        <v>45672</v>
+      </c>
+      <c r="G131" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H131" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B142" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C142" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D142" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E142" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>